<commit_message>
Ignore hidden Excel and CSV files in backend
</commit_message>
<xml_diff>
--- a/backend/audit_logs.xlsx
+++ b/backend/audit_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,6 +564,670 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-12-28 00:12:09</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>gemini-3-flash-preview</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+EX-10 2 tmb-20250626xex10.htm EX-10
+FIRST AMENDMENT TO AMENDED AND RESTATED CREDIT
+AGREEMENT
+FIRST AMENDMENT TO AMENDED AND RESTATED CREDIT AGREEMENT
+(this “Agreement”), dated as of June 26, 2025 (and effective as set forth below), among
+MAYVILLE ENGINEERING COMPANY, INC., a Wisconsin corporation (the “Borrower”),
+the Subsidiary Guarantors (as defined in the Existing Credit Agreement referred to below)
+party hereto, the Incremental Lenders (as defined below), the Lenders (as defined below)
+party hereto (the “Consenting Lenders”), and WELLS FARGO BANK, NATIONAL
+ASSOCIATION, as administrative agent (the “Administrative Agent”). Unless otherwise
+indicated, all capitalized terms used herein and not otherwise defined herein shall have the
+respective meanings provided such terms in the Credit Agreement referred to below.
+W I T N E S S E T H:
+WHEREAS, the Borrower, the lenders party thereto (the “Lenders”) and the
+Administrative Agent have entered into that certain Amended and Restated Credit Agreement,
+dated as of June 28, 2023 (as amended, restated, supplemented or otherwise modified prior to
+the date hereof, the “Existing Credit Agreement” and as hereby amended and as from time to
+time further amended, modified, supplemented, restated, or amended and restated, the “Credit
+Agreement”);
+WHEREAS, the Borrower has requested an Incremental Revolving Credit Increase in
+the aggregate principal amount of $100,000,000, in accordance with Section 5.13 of the
+Existing Credit Agreement (the “First Amendment Revolving Credit Increase”);
+WHEREAS, subject to the terms of this Agreement, certain of the Revolving Credit
+Lenders identified on the signature pages hereto (each an “Incremental Lender”) are severally
+willing to provide a portion of the First Amendment Revolving Credit Increase; and
+WHEREAS, the Borrower has also requested, and subject to the terms and conditions
+set forth herein, the Administrative Agent and the Consenting Lenders have agreed to further
+amend the Existing Credit Agreement as more specifically set forth herein.
+NOW, THEREFORE, in consideration of the foregoing and for other good and
+valuable consideration, the receipt and sufficiency of which are hereby acknowledged, it is
+agreed as follows:
+SECTION 1.Amendments to Existing Credit Agreement. Effective as of the First
+Amendment Effective Date (as defined below) and subject to the terms and conditions set
+forth herein and in reliance upon the representations and warranties set forth herein:
+(a)Schedule 1.1 (Commitments and Commitment Percentages) to the Existing
+Credit Agreement is hereby amended and restated in the form attached hereto
+as Annex A.
+(b)the body of Existing Credit Agreement is hereby amended as follows: (i) to
+delete red or green stricken text (indicated textually in the same manner as the
+following examples: stricken text and stricken text) and (ii) to add the blue or
+green double-underlined text (indicated textually in the same manner as the
+following examples: double-underlined text and double-underlined text), in
+each case, as set forth in the conformed copy attached hereto as Annex B.1SECTION 2.Revolving Credit Facility Increase; Reallocation.
+(a)Each Incremental Lender severally agrees that its Revolving Credit
+Commitment after giving effect to the First Amendment Revolving Credit
+Increase shall be as set forth opposite such Lender’s name on Annex A hereto.
+(b)The parties hereto hereby agree that (i) this Agreement constitutes a request
+for an Incremental Revolving Credit Increase pursuant to Section 5.13 of the
+Credit Agreement, (ii) the parties hereto hereby waive any prior notice
+required thereby, and (iii) this Agreement shall be deemed to be an “Lender
+Joinder Agreement” in accordance with Section 5.13(h) of the Credit
+Agreement.
+(c)Pursuant to Section 5.13 of the Credit Agreement, on the First Amendment
+Effective Date (as defined below) and after giving effect to this Agreement,
+the outstanding Revolving Credit Loans and Revolving Credit Commitment
+Percentages of Swingline Loans and L/C Obligations will be reallocated by
+the Administrative Agent among the Revolving Credit Lenders (including the
+Incremental Lenders providing the First Amendment Revolving Credit
+Increase) in accordance with their revised Revolving Credit Commitment
+Percentages (and the Revolving Credit Lenders (including the Incremental
+Lenders providing the First Amendment Revolving Credit Increase) agree to
+make all payments and adjustments necessary to effect such reallocation and
+the Borrower shall pay any and all costs required pursuant to Section 5.9 of
+the Credit Agreement in connection with such reallocation as if such
+reallocation were a repayment).
+SECTION 3.Conditions of Effectiveness of this Agreement.  This Agreement shall
+become effective on the date when the following conditions shall have been satisfied or
+waived (such date, the “First Amendment Effective Date”):
+(a) The Administrative Agent’s receipt of the following, each in form and
+substance reasonably satisfactory to the Administrative Agent:
+(i) this Agreement, duly executed by each of the Credit Parties existing
+as of the First Amendment Effective Date, the Administrative Agent, each
+Incremental Lender and each of the Consenting Lenders;
+(ii) a certificate of a Responsible Officer (or the secretary or assistant
+secretary) of each Credit Party certifying as to the incumbency and genuineness of the
+signature of each officer of such Credit Party executing Loan Documents to which it
+is a party and certifying that attached thereto is a true, correct and complete copy of
+(A) the articles or certificate of incorporation or formation (or equivalent), as
+applicable, of such Credit Party and all amendments thereto, certified as of a recent
+date by the appropriate Governmental Authority in its jurisdiction of incorporation,
+organization or formation (or equivalent), as applicable, (B) the bylaws or other
+governing document of such Credit Party as in effect on the First Amendment
+Effective Date, (C) resolutions duly adopted by the board of directors (or other
+governing body) of such Credit Party authorizing and approving the transactions
+contemplated hereunder and the execution, delivery and performance of this
+Amendment, the Credit Agreement and the other Loan Documents to which it is a
+party, and (D) certificates as of a recent date of the good standing of each Credit Party2under the laws of its jurisdiction of incorporation, organization or formation (or
+equivalent), as applicable;
+(iii) an Officer’s Compliance Certificate demonstrating, in form and
+substance reasonably satisfactory to the Administrative Agent, that the Borrower is in
+compliance with thefinancial covenants set forth in Section 9.15 of the Credit Agreement as of the First
+Amendment Effective Date based on the financial statements most recently delivered
+pursuant to Section 8.1(a) or 8.1(b) of the Existing Credit Agreement, as applicable,
+both before and after giving effect (on a pro forma basis) to (x) any Incremental
+Revolving Credit Commitment, and (y) the making of the First Amendment
+Revolving Credit Increase pursuant thereto (with such Incremental Revolving Credit
+Commitment being deemed to be fully funded);
+(iv) a certificate from the chief financial officer of the Borrower with
+respect to solvency (on a consolidated basis) of the Borrower and its Subsidiaries as
+of the First Amendment Effective Date after giving effect to the First Amendment
+Revolving Credit Increase and the other amendments contemplated by this
+Agreement;
+(v) an opinion from counsel to the Credit Parties, in form and substance
+reasonably satisfactory to the Administrative Agent.
+(b) The representations and warranties set forth in Section 3 shall be true and
+correct.
+(c) No Default or Event of Default shall exist on the First Amendment Effective
+Date immediately prior to or after giving effect to this Agreement.
+(d) The Administrative Agent shall have received the results of a Lien search, in
+form and substance reasonably satisfactory thereto, made against the Credit Parties under the
+Uniform Commercial Code (or applicable judicial docket) as in effect in each jurisdiction in
+which filings or recordations under the Uniform Commercial Code should be made to
+evidence or perfect security interests in all assets of such Credit Party, indicating among other
+things that the assets of each such Credit Party are free and clear of any Lien (except for
+Permitted Liens).
+(e) All governmental, shareholder and third party consents and approvals
+necessary (or any other material consents as determined in the reasonable discretion of the
+Administrative Agent) in connection with the transactions contemplated by this Agreement
+shall have been obtained and shall be in full force and effect.
+(f) The Borrower and each of the Subsidiary Guarantors shall have provided to
+the Administrative Agent and the Lenders, at least five (5) Business Days prior to the First
+Amendment Effective Date, a Beneficial Ownership Certification under 31 C.F.R. 1010.230
+and all documentation and other information required by regulatory authorities under
+applicable “know your customer”, anti-money-laundering, beneficial ownership and other
+similar rules and regulations, including, without limitation, the PATRIOT Act.
+(g) The Borrower shall have paid all fees and expenses required to be paid on the
+First Amendment Effective Date.
+For purposes of determining compliance with the conditions specified in this Section 3, the
+Administrative Agent, each Incremental Lender and each Consenting Lender that has signed
+this Agreement shall be deemed to have consented to, approved or accepted or to be satisfied
+with, each document or other matter required thereunder to be consented to or approved by or
+acceptable or satisfactory to an Incremental Lender and/or a Consenting Lender, as applicable,
+unless the Administrative Agent shall have received notice from such Incremental Lender3and/or Consenting Lender, as applicable, prior to the proposed First Amendment Effective
+Date specifying its objection thereto.SECTION 4.Representations and Warranties.  To induce the Administrative Agent,
+the Incremental Lenders party hereto and the Consenting Lenders party hereto to enter into
+this Agreement, each Credit Party represents and warrants to the Administrative Agent, the
+Incremental Lenders and the Consenting Lenders on and as of the First Amendment Effective
+Date that, in each case:
+(a) each of the representations and warranties contained in Article VII of the
+Credit Agreement are true and correct in all material respects, except to the extent any such
+representation and warranty is qualified by materiality or reference to Material Adverse
+Effect, in which case, such representation and warranty is true, correct and complete in all
+respects, with the same effect as if made on and as of such date (except for any such
+representation and warranty that by its terms is made only as of an earlier date, which
+representation and warranty remains true and correct as of such earlier date);
+(b) no Default or Event of Default has occurred and is continuing immediately
+prior to or after giving effect to this Agreement;
+(c) it has the right, power and authority and has taken all necessary corporate and
+other action to authorize the execution, delivery and performance of this Agreement in
+accordance with their respective terms; and
+(d) this Agreement has been duly executed and delivered by the duly authorized
+officers, managers, managing members or other authorized person of each Credit Party that is
+a party thereto, and each such document constitutes the legal, valid and binding obligation of
+each Credit Party, enforceable in accordance with its terms, except as such enforceability may
+be limited by bankruptcy, insolvency, reorganization, moratorium or similar state or federal
+Debtor Relief Laws from time to time in effect which affect the enforcement of creditors’
+rights in general and the availability of equitable remedies.
+SECTION 5.Credit Party Acknowledgements, Agreements and Confirmations.  By
+its execution of this Agreement, each Credit Party hereby (a) consents to this Agreement and
+agrees that the transactions contemplated by this Agreement shall not limit or diminish the
+obligations of such Credit Party, or release such Credit Party from any obligations, under any
+of the Loan Documents to which it is a party, (b) confirms and reaffirms its obligations under
+each of the Loan Documents to which it is a party and (c) agrees that each of the Loan
+Documents to which it is a party remain in full force and effect and are hereby ratified and
+confirmed.
+SECTION 6.Reference to and Effect on the Credit Agreement and the Loan
+Documents.
+(a) On and after the First Amendment Effective Date, each reference in the Credit
+Agreement to “this Agreement,” “herein,” “hereto”, “hereof” and “hereunder” or words of like
+import referring to the Credit Agreement, and each reference in the Notes and each of the
+other Loan Documents to “the Credit Agreement”, “thereunder”, “thereof” or words of like
+import referring to the Credit Agreement, shall mean and be a reference to the Credit
+Agreement, as amended and supplemented by this Agreement.
+(b) The Credit Agreement and each of the other Loan Documents, as specifically
+amended and supplemented by this Agreement, are and shall continue to be in full force and
+effect and are hereby in all respects ratified and confirmed.
+(c) The execution, delivery and effectiveness of this Agreement shall not, except
+as expressly provided herein, operate as a waiver of any right, power or remedy of any Lender
+or the Administrative Agent under any of the Loan Documents, nor constitute a waiver of any
+provision of any of the Loan Documents.  Without limiting the generality of the foregoing, the4Security Documents in effect immediately prior to the date hereof and all of the Collateral
+described therein in existence immediately prior to the date hereof do and shall continue to
+secure the payment of all Secured Obligations.  5(d) This Agreement is the entire agreement, and supersedes any prior agreements
+and contemporaneous oral agreements, of the parties concerning its subject matter. This
+Agreement shall constitute a “Loan Document” for all purposes of the Credit Agreement and
+the other Loan Documents.
+(e) This Agreement shall be binding on and inure to the benefit of the parties
+hereto and their successors and permitted assigns.
+SECTION 7.Costs and Expenses.  The Borrower hereby reconfirms its obligations
+pursuant to Section 12.3 of the Credit Agreement to pay and reimburse the Administrative
+Agent for all reasonable fees, costs and expenses in accordance with the terms thereof.
+SECTION 8.Governing Law; Jury Trial Waiver.  This Agreement and any claim,
+controversy, dispute or cause of action (whether in contract or tort or otherwise) based upon,
+arising out of or relating to this Agreement and the transactions contemplated hereby shall be
+governed by, and construed in accordance with, the law of the State of New York.  EACH
+PARTY HERETO HEREBY IRREVOCABLY WAIVES, TO THE FULLEST EXTENT
+PERMITTED BY APPLICABLE LAW, ANY RIGHT IT MAY HAVE TO A TRIAL BY JURY
+IN ANY LEGAL PROCEEDING DIRECTLY OR INDIRECTLY ARISING OUT OF OR
+RELATING TO THIS AGREEMENT OR THE TRANSACTIONS CONTEMPLATED
+HEREBY (WHETHER BASED ON CONTRACT, TORT OR ANY OTHER THEORY).  EACH
+PARTY HERETO (A) CERTIFIES THAT NO REPRESENTATIVE, AGENT OR ATTORNEY
+OF ANY OTHER PERSON HAS REPRESENTED, EXPRESSLY OR OTHERWISE, THAT
+SUCH OTHER PERSON WOULD NOT, IN THE EVENT OF LITIGATION, SEEK TO
+ENFORCE THE FOREGOING WAIVER AND (B) ACKNOWLEDGES THAT IT AND THE
+OTHER PARTIES HERETO HAVE BEEN INDUCED TO ENTER INTO THIS AGREEMENT
+BY, AMONG OTHER THINGS, THE MUTUAL WAIVERS AND CERTIFICATIONS IN THIS
+SECTION.
+SECTION 9.Counterparts; Electronic Execution. This Agreement may be executed
+in counterparts (and by different parties hereto in different counterparts), each of which shall
+constitute an original, but all of which when taken together shall constitute a single contract.
+Delivery of an executed counterpart of a signature page of this Agreement by facsimile or in
+electronic (i.e., “pdf” or “tif”) format shall be effective as delivery of a manually executed
+counterpart of this Agreement. This Agreement may be executed by Electronic Signatures or
+in the form of an Electronic Record pursuant to, and in accordance with, the provisions of
+Section 12.16 of the Credit Agreement.
+[Signature pages to follow]Mayville Engineering Company, Inc.IN WITNESS WHEREOF, the parties hereto have caused their duly authorized
+officers to execute and deliver this Agreement as of the date first above written.
+BORROWER:
+MAYVILLE ENGINEERING COMPANY,
+INC.
+SUBSIDIARY GUARANTORS:
+CENTER MANUFACTURING
+HOLDINGS, INC.
+CENTER MANUFACTURING, INC.
+CENTER – MOELLER PRODUCTS LLC
+DEFIANCE METAL PRODUCTS CO.
+DEFIANCE METAL PRODUCTS OF
+ARKANSAS, INC. 
+ By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageMayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageDEFIANCE METAL PRODUCTS OF PA.,
+INC.
+MID-STATES ALUMINUM, LLC 
+ By:
+Name:
+Title:
+By:
+Name:
+Title:Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageWELLS FARGO BANK, NATIONAL
+ASSOCIATION, as Administrative Agent,
+Issuing Lender, Swingline Lender,
+Consenting Lender and an Incremental
+Lender
+By:
+___________________________________
+Name:
+Title:  Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageJPMORGAN CHASE BANK, N.A., as a
+Consenting Lender and an Incremental
+Lender
+By:
+___________________________________
+Name:
+Title:  Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageTD BANK, N.A., as a Consenting Lender
+and an Incremental Lender
+By:
+___________________________________
+Name:
+Title:  Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageCITIBANK, N.A., as a Consenting Lender
+By:
+___________________________________
+Name:
+Title:  Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageHANMI BANK, as a Consenting Lender and
+an Incremental Lender
+By:
+___________________________________
+Name:
+Title:  Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageASSOCIATED BANK, N.A., as a
+Consenting Lender and an Incremental
+Lender
+By:
+___________________________________
+Name:
+Title:  Annex A
+REVOLVING CREDIT COMMITMENTS AND REVOLVING CREDIT COMMITMENT
+PERCENTAGES
+Lender Revolving
+Credit
+CommitmentRevolving
+Credit
+Commitment
+Percentage
+Wells Fargo Bank, National
+Association 
+$108,000,000.00 30.857142858%
+JPMorgan Chase Bank, N.A.  $90,000,000.00 25.714285714%
+TD Bank, N.A.  $77,000,000.00 22.000000000%
+Associated Bank, N.A.  $30,000,000.00 8.571428571%
+Hanmi Bank  $25,000,000.00 7.142857143%
+Citibank, N.A.  $20,000,000.00 5.714285714%
+Total $350,000,000.00100.000000000%ANNEX B
+Published CUSIP Number: 57859VAP8
+$350,000,000.00
+AMENDED AND RESTATED CREDIT AGREEMENT
+dated as of June 28, 2023
+(as amended by that certain First Amendment to Amended and Restated Credit Agreement
+dated as of June 26, 2025)
+by and among
+MAYVILLE ENGINEERING COMPANY, INC.
+as Borrower,
+the Lenders referred to herein,
+as Lenders,
+and
+WELLS FARGO BANK, NATIONAL ASSOCIATION,
+as Administrative Agent,
+Swingline Lender and Issuing Lender
+and
+WELLS FARGO SECURITIES, LLC,
+as Joint Lead Arranger and Joint Bookrunner
+and
+J.P. MORGAN SECURITIES LLC,
+as Joint Lead Arranger and Joint Bookrunner
+and
+TD BANK, N.A.,
+as Joint Lead Arranger and Joint Bookrunner i 
+ ARTICLE IDEFINITIONS 1
+SECTION 1.1Definitions 1
+SECTION 1.2Other Definitions and Provisions 31
+SECTION 1.3Accounting Terms 31
+SECTION 1.4UCC Terms 32
+SECTION 1.5Rounding 32
+SECTION 1.6References to Agreement and Laws 32
+SECTION 1.7Times of Day 32
+SECTION 1.8Letter of Credit Amounts 32
+SECTION 1.9Guarantees/Earn-Outs 33
+SECTION 1.10Covenant Compliance Generally 33
+SECTION 1.11Rates 33
+SECTION 1.12Divisions 33
+ARTICLE IIREVOLVING CREDIT FACILITY 34
+SECTION 2.1Revolving Credit Loans 34
+SECTION 2.2Swingline Loans 34
+SECTION 2.3Procedure for Advances of Revolving Credit Loans and Swingline
+Loans 36
+SECTION 2.4Repayment and Prepayment of Revolving Credit Loans and Swingline
+Loans 37
+SECTION 2.5Permanent Reduction of the Revolving Credit Commitment 37
+SECTION 2.6Termination of Revolving Credit Facility 38
+ARTICLE IIILETTER OF CREDIT FACILITY 38
+SECTION 3.1L/C Facility 38
+SECTION 3.2Procedure for Issuance of Letters of Credit 39
+SECTION 3.3Commissions and Other Charges 39
+SECTION 3.4L/C Participations 40
+SECTION 3.5Reimbursement Obligation of the Borrower 41
+SECTION 3.6Obligations Absolute 41
+SECTION 3.7Effect of Letter of Credit Application 41
+SECTION 3.8Resignation of Issuing Lenders 42
+SECTION 3.9Reporting of Letter of Credit Information and L/C Commitment 42
+SECTION 3.10Letters of Credit Issued for Subsidiaries 42ii 
+ ARTICLE IVReserved 43
+ARTICLE VGENERAL LOAN PROVISIONS 43
+SECTION 5.1Interest 43
+SECTION 5.2Notice and Manner of Conversion or Continuation of Loans 44
+SECTION 5.3Fees 44
+SECTION 5.4Manner of Payment 45
+SECTION 5.5Evidence of Indebtedness 45
+SECTION 5.6Sharing of Payments by Lenders 46
+SECTION 5.7Administrative Agent’s Clawback 46
+SECTION 5.8Changed Circumstances 47
+SECTION 5.9Indemnity 50
+SECTION 5.10Increased Costs 50
+SECTION 5.11Taxes 51
+SECTION 5.12Mitigation Obligations; Replacement of Lenders 55
+SECTION 5.13Incremental Loans 56
+SECTION 5.14Cash Collateral 58
+SECTION 5.15Defaulting Lenders 58
+ARTICLE VICONDITIONS OF CLOSING AND BORROWING 60
+SECTION 6.1Conditions to Closing and Initial Extensions of Credit 60
+SECTION 6.2Conditions to All Extensions of Credit 64
+ARTICLE VIIREPRESENTATIONS AND WARRANTIES OF THE CREDIT PARTIES64
+SECTION 7.1Organization; Power; Qualification 64
+SECTION 7.2Ownership 65
+SECTION 7.3Authorization; Enforceability 65
+SECTION 7.4Compliance of Agreement, Loan Documents and Borrowing with
+Laws, Etc 65
+SECTION 7.5Compliance with Law; Governmental Approvals 65
+SECTION 7.6Tax Returns and Payments 66
+SECTION 7.7Intellectual Property Matters 66
+SECTION 7.8Environmental Matters 66
+SECTION 7.9Employee Benefit Matters 67
+SECTION 7.10Margin Stock 68
+SECTION 7.11Government Regulation 68
+SECTION 7.12Material Contracts 68
+SECTION 7.13Employee Relations 68iii 
+ SECTION 7.14Burdensome Provisions 69
+SECTION 7.15Financial Statements 69
+SECTION 7.16No Material Adverse Change 69
+SECTION 7.17Solvency 69
+SECTION 7.18Title to Properties 69
+SECTION 7.19Litigation 69
+SECTION 7.20Anti-Corruption Laws; Anti-Money Laundering Laws; Sanctions and
+Outbound Investment Rules 69
+SECTION 7.21Absence of Defaults 70
+SECTION 7.22ESOP 70
+SECTION 7.23Senior Indebtedness Status 71
+SECTION 7.24Disclosure 71
+ARTICLE VIIIAFFIRMATIVE COVENANTS 72
+SECTION 8.1Financial Statements and Budgets 72
+SECTION 8.2Certificates; Other Reports 73
+SECTION 8.3Notice of Litigation and Other Matters 73
+SECTION 8.4Preservation of Corporate Existence and Related Matters 75
+SECTION 8.5Maintenance of Property and Licenses 75
+SECTION 8.6Insurance 75
+SECTION 8.7Accounting Methods and Financial Records 76
+SECTION 8.8Payment of Taxes and Other Obligations 76
+SECTION 8.9Compliance with Laws and Approvals 76
+SECTION 8.10Environmental Laws 76
+SECTION 8.11Compliance with ERISA 76
+SECTION 8.12Compliance with Material Contracts 76
+SECTION 8.13Visits and Inspections 76
+SECTION 8.14Additional Subsidiaries 77
+SECTION 8.15Depository Bank 77
+SECTION 8.16Use of Proceeds 78
+SECTION 8.17ESOP 78
+SECTION 8.18Compliance with Anti-Corruption Laws; Beneficial Ownership
+Regulation, Anti-Money Laundering Laws and Sanctions 78
+SECTION 8.19Further Assurances 78
+SECTION 8.20Post-Closing Matters 79
+SECTION 8.21Lender Meetings 79iv 
+ ARTICLE IXNEGATIVE COVENANTS 79
+SECTION 9.1Indebtedness 79
+SECTION 9.2Liens 80
+SECTION 9.3Investments 81
+SECTION 9.4Fundamental Changes 82
+SECTION 9.5Asset Dispositions 83
+SECTION 9.6Restricted Payments 84
+SECTION 9.7Transactions with Affiliates 84
+SECTION 9.8Accounting Changes; Organizational Documents 84
+SECTION 9.9Payments and Modifications of Subordinated Indebtedness 85
+SECTION 9.10No Further Negative Pledges; Restrictive Agreements 85
+SECTION 9.11ESOP Matters 86
+SECTION 9.12Sale of Accounts 86
+SECTION 9.13Sale Leasebacks 86
+SECTION 9.14Capital Expenditures 86
+SECTION 9.15Financial Covenants 86
+SECTION 9.16No Amendment to ESOP Documentation 87
+SECTION 9.17Limitations Regarding Outbound Investment Rules 87
+ARTICLE XDEFAULT AND REMEDIES 87
+SECTION 10.1Events of Default 87
+SECTION 10.2Remedies 89
+SECTION 10.3Rights and Remedies Cumulative; Non-Waiver; etc 90
+SECTION 10.4Crediting of Payments and Proceeds 91
+SECTION 10.5Administrative Agent May File Proofs of Claim 91
+SECTION 10.6Credit Bidding 92
+ARTICLE XITHE ADMINISTRATIVE AGENT 92
+SECTION 11.1Appointment and Authority 92
+SECTION 11.2Rights as a Lender 93
+SECTION 11.3Exculpatory Provisions 93
+SECTION 11.4Reliance by the Administrative Agent 94
+SECTION 11.5Delegation of Duties 94
+SECTION 11.6Resignation of Administrative Agent 95
+SECTION 11.7Non-Reliance on Administrative Agent and Other Lenders 96
+SECTION 11.8No Other Duties, Etc 96
+SECTION 11.9Collateral and Guaranty Matters 96v 
+ SECTION 11.10Secured Hedge Agreements and Secured Cash Management
+Agreements 97
+SECTION 11.11[Reserved.] 97
+SECTION 11.12Erroneous Payments 97
+ARTICLE XIIMISCELLANEOUS 99
+SECTION 12.1Notices 99
+SECTION 12.2Amendments, Waivers and Consents 101
+SECTION 12.3Expenses; Indemnity 103
+SECTION 12.4Right of Setoff 105
+SECTION 12.5Governing Law; Jurisdiction, Etc 105
+SECTION 12.6Waiver of Jury Trial 106
+SECTION 12.7Reversal of Payments 106
+SECTION 12.8Injunctive Relief 107
+SECTION 12.9Successors and Assigns; Participations 107
+SECTION 12.10Treatment of Certain Information; Confidentiality 110
+SECTION 12.11Performance of Duties 111
+SECTION 12.12All Powers Coupled with Interest 111
+SECTION 12.13Survival 111
+SECTION 12.14Titles and Captions 112
+SECTION 12.15Severability of Provisions 112
+SECTION 12.16Counterparts; Integration; Effectiveness; Electronic Execution 112
+SECTION 12.17Term of Agreement 113
+SECTION 12.18USA PATRIOT Act; Anti-Money Laundering Laws 113
+SECTION 12.19Independent Effect of Covenants 113
+SECTION 12.20No Advisory or Fiduciary Responsibility 113
+SECTION 12.21Amendment and Restatement; No Novation 114
+SECTION 12.22Inconsistencies with Other Documents 115
+SECTION 12.23Acknowledgement and Consent to Bail-In of Affected Financial
+Institutions 115
+SECTION 12.24Certain ERISA Matters 115
+SECTION 12.25Acknowledgement Regarding Any Supported QFCs 116viEXHIBITS
+Exhibit A-1 -Form of Revolving Credit Note
+Exhibit A-2 -Form of Swingline Note
+Exhibit B -Form of Notice of Borrowing
+Exhibit C -Form of Notice of Account Designation
+Exhibit D -Form of Notice of Prepayment
+Exhibit E -Form of Notice of Conversion/Continuation
+Exhibit F -Form of Officer’s Compliance Certificate
+Exhibit G -Form of Assignment and Assumption
+Exhibit H-1 -Form of U.S. Tax Compliance Certificate (Non-
+Partnership Foreign Lenders)
+Exhibit H-2 -Form of U.S. Tax Compliance Certificate (Non-
+Partnership Foreign Participants)
+Exhibit H-3 -Form of U.S. Tax Compliance Certificate (Foreign
+Participant Partnerships)
+Exhibit H-4 -Form of U.S. Tax Compliance Certificate (Foreign Lender
+Partnerships)
+Exhibit I -Form of Joinder Agreement
+SCHEDULES
+Schedule 1.1 -Commitments and Commitment Percentages
+Schedule 7.1 -Jurisdictions of Organization and Qualification
+Schedule 7.2 -Subsidiaries and Capitalization
+Schedule 7.6 -Tax Matters
+Schedule 7.9 -ERISA Plans
+Schedule 7.12 -Material Contracts
+Schedule 7.13 -Labor and Collective Bargaining Agreements
+Schedule 7.18 -Real Property
+Schedule 7.19 -Litigation
+Schedule 8.20 -Post-Closing Matters
+Schedule 9.1 -Existing Indebtedness
+Schedule 9.2 -Existing Liens
+Schedule 9.3 -Existing Loans, Advances and Investments
+Schedule 9.7 -Transactions with Affiliates
+Schedule 12.21 -Existing Letters of CreditAMENDED AND RESTATED CREDIT AGREEMENT, dated as of June 28, 2023, by and
+among MAYVILLE ENGINEERING COMPANY, INC., a Wisconsin corporation (“Mayville” or the
+“Borrower”), the lenders who are party to this Agreement and the lenders who may become a party to
+this Agreement pursuant to the terms hereof, as Lenders, and WELLS FARGO BANK, NATIONAL
+ASSOCIATION, a national banking association, as Administrative Agent for the Lenders.
+STATEMENT OF PURPOSE
+The Borrower, the lenders party thereto, and WELLS FARGO BANK, NATIONAL
+ASSOCIATION, a national banking association, as administrative agent for such lenders, are party to
+that certain Amended and Restated Credit Agreement dated as of September 26, 2019 (as amended to
+date, the “Existing Credit Agreement”).  
+The Borrower has requested, and subject to the terms and conditions set forth in this
+Agreement, the Administrative Agent and the Lenders have agreed to extend certain credit facilities
+to the Borrower to be used, in part, to restructure, and to increase, the indebtedness and other
+obligations outstanding under the Existing Credit Agreement and amend and restate the Existing
+Credit Agreement in its entirety.
+NOW, THEREFORE, for good and valuable consideration, the receipt and sufficiency of
+which are hereby acknowledged by the parties hereto, such parties hereby agree as follows:
+ARTICLE I
+DEFINITIONS
+SECTION 1.1 Definitions.  The following terms when used in this Agreement shall
+have the meanings assigned to them below:
+“Accu-Fab Acquisition” means the contemplated Acquisition by the Borrower of all of the
+outstanding Equity Interests of Accu-Fab, LLC, a Delaware limited liability company, from Tide
+Rock Yieldco, LLC, a Delaware limited liability company, pursuant to that certain Purchase
+Agreement, dated as of May 23, 2025, by and among the Borrower, Accu-Fab, LLC and Tide Rock
+Yieldco, LLC.  
+“Acquisition” means any transaction, or any series of related transactions, consummated on
+or after the date of this Agreement, by which any Credit Party or any of its Subsidiaries (a) acquires
+any business or all or substantially all of the assets of any Person, or division thereof, whether
+through purchase of assets, merger or otherwise or (b) directly or indirectly acquires (in one
+transaction or as the most recent transaction in a series of transactions) at least a majority (in number
+of votes) of the securities of a corporation which have ordinary voting power for the election of
+members of the board of directors or the equivalent governing body (other than securities having
+such power only by reason of the happening of a contingency) or a majority (by percentage or voting
+power) of the outstanding ownership interests of a partnership or limited liability company.
+“Administrative Agent” means Wells Fargo, in its capacity as Administrative Agent
+hereunder, and any successor thereto appointed pursuant to Section 11.6.
+“Administrative Agent’s Office” means the office of the Administrative Agent specified in or
+determined in accordance with the provisions of Section 12.1(c).
+“Administrative Questionnaire” means an administrative questionnaire in</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, Section 1(b)",
+      "error": "The document references a conformed copy showing deletions and additions in 'Annex B.1', but the attached annex is labeled 'ANNEX B' and is a clean (non-marked) document.",
+      "suggestion": "Ensure the attachment is either relabeled to match the text or that a redlined version is provided if that was the intent of Section 1(b)."
+    },
+    {
+      "location": "Page 2, Section 3(a)(iii)",
+      "error": "Scrivener's error: 'thefinancial' is missing a space between the words.",
+      "suggestion": "Correct to 'the financial'."
+    },
+    {
+      "location": "Annex B, Section 1.1, Definition of 'Accu-Fab Acquisition'",
+      "error": "The term 'Purchase Agreement' is capitalized and used as a specific deal-related defined term but is not defined within the 'Definitions' section or elsewhere in the document fragment.",
+      "suggestion": "Define 'Purchase Agreement' or use a more specific defined term (e.g., 'Accu-Fab Purchase Agreement') and cross-reference its definition."
+    },
+    {
+      "location": "Annex B, Section 1.1, Definition of 'Applicable Margin' Table",
+      "error": "Pricing Level I of the 'Consolidated Total Leverage Ratio' column lacks the 'to 1.00' ratio suffix, which is inconsistent with the formatting used in Pricing Levels II through V.",
+      "suggestion": "Update Pricing Level I to read 'Greater than or equal to 3.25 to 1.00'."
+    },
+    {
+      "location": "Annex B, Section 1.1, Definition of 'MSA Acquisition'",
+      "error": "The term 'Unit Purchase Agreement' is capitalized and used as a specific deal-related defined term but is not defined within the 'Definitions' section.",
+      "suggestion": "Define 'Unit Purchase Agreement' or provide a specific reference to the acquisition document."
+    },
+    {
+      "location": "Signature Pages (Multiple)",
+      "error": "Drafting placeholders: The 'By', 'Name', and 'Title' fields are blank for the Borrower, all Subsidiary Guarantors, and all Lenders.",
+      "suggestion": "Populate all signature blocks with the names and titles of the authorized signatories."
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance PDF extraction logic and update project logs
</commit_message>
<xml_diff>
--- a/backend/audit_logs.xlsx
+++ b/backend/audit_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1228,6 +1228,124 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-12-28 01:13:43</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>gemini-3-flash-preview</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, Article I, Definition of 'Applicable Margin'",
+      "error": "Mathematical logic gap in pricing grid. The range between 2.50 to 1.00 and 2.60 to 1.00 is not covered. Level II starts at 2.60 while Level III ends at 2.50.",
+      "suggestion": "Adjust the Consolidated Total Leverage Ratio for Pricing Level II to 'Greater than or equal to 2.50 to 1.00 but less than 3.25 to 1.00' to ensure continuity."
+    },
+    {
+      "location": "Page 1, Section 2.5",
+      "error": "The term 'Cash Collateralization' is used but is explicitly noted as being undefined in the document.",
+      "suggestion": "Add a definition for 'Cash Collateralization' in Article I or replace the usage with the defined term 'Cash Collateral'."
+    },
+    {
+      "location": "Page 2, Section 5.13",
+      "error": "Drafting placeholder '[__]' found in the notice delivery provision.",
+      "suggestion": "Replace '[__]' with the specific physical location or city of the Administrative Agent's office."
+    },
+    {
+      "location": "Page 2, Section 5.13",
+      "error": "Internal cross-reference to 'Section 5.19' cannot be verified as the section is missing from the document.",
+      "suggestion": "Confirm that Section 5.19 exists in the full agreement or update the reference to the correct section."
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement structured audit errors and ErrorListPanel UI
</commit_message>
<xml_diff>
--- a/backend/audit_logs.xlsx
+++ b/backend/audit_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,6 +1705,129 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-29 22:50:01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>gemini-3-flash-preview</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, Article I, 'Applicable Margin' table",
+      "error": "Mathematical/logical gap in pricing levels: Level II ends at '2.60 to 1.00' and Level III starts at '2.50 to 1.00'. A ratio between 2.50 and 2.60 (e.g., 2.55) is not covered.",
+      "suggestion": "Change Level III to 'Greater than or equal to 1.75 to 1.00 but less than 2.60 to 1.00'."
+    },
+    {
+      "location": "Page 1, Section 2.5",
+      "error": "The term 'Cash Collateralization' is used but is not defined in the Article I definitions section (as noted in the parenthetical within Article I).",
+      "suggestion": "Add a definition for 'Cash Collateralization' or replace with the term 'Cash Collateral'."
+    },
+    {
+      "location": "Page 2, Section 5.13",
+      "error": "Drafting placeholder '[__]' remains in the text regarding the location of the Administrative Agent's office.",
+      "suggestion": "Replace the placeholder with the appropriate city, state, or specific address."
+    },
+    {
+      "location": "Page 2, Section 5.13",
+      "error": "The term 'Incremental Revolving Credit Increase' is capitalized and used as a specific instrument/action but is not defined in this document.",
+      "suggestion": "Define 'Incremental Revolving Credit Increase' in Article I or within Section 5.13."
+    },
+    {
+      "location": "Page 2, Section 5.13",
+      "error": "Internal cross-reference to 'Section 5.19' appears to be broken as the document fragment ends at Section 5.13.",
+      "suggestion": "Verify if the documentation requirements should refer to a section within this Amendment or a section in the base Credit Agreement."
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added parallel worker, many locators, to help locate exact coordinates on the PDF based on error info gathered before
</commit_message>
<xml_diff>
--- a/backend/audit_logs.xlsx
+++ b/backend/audit_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2070,6 +2070,1728 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-30 00:49:42</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+ EX-4.1 3 d45101 1dex41.htm EX-4.1 
+ Exhibit 4.1 
+ CAPIT AL ONE PRIME AUT O RECEIV ABLES TRUST 2023-1 
+ Class A-1 4.900% Auto Loan Asset Backed Notes 
+ Class A-2 5.20% Auto Loan Asset Backed Notes 
+ Class A-3 4.87% Auto Loan Asset Backed Notes 
+ Class A-4 4.76% Auto Loan Asset Backed Notes 
+ Class B 5.07% Auto Loan Asset Backed Notes 
+ Class C 5.36% Auto Loan Asset Backed Notes 
+ Class D 6.34% Auto Loan Asset Backed Notes 
+ INDENTURE 
+ Dated as of February 23, 2023 
+ WILMINGT ON TRUST , NATIONAL ASSOCIA TION, 
+ as the Indenture T rustee 
+--- [START OF PAGE 2] ---
+ CROSS REFERENCE T ABLE  1 
+ TIA  Section  Indenture  Section 
+ 310  (a) (1)  6.11 
+ (a) (2)  6.11 
+ (a) (3)  6.10; 6.1 1 
+ (a) (4)  N.A.  2 
+ (a) (5)  6.11 
+ (b)  6.8; 6.1 1 
+ (c)  N.A. 
+ 311  (a)  6.12 
+ (b)  6.12 
+ (c)  N.A. 
+ 312  (a)  7.1 
+ (b)  7.2 
+ (c)  7.2 
+ 313  (a)  7.3 
+ (b) (1)  7.3 
+ (b) (2)  7.3 
+ (c)  7.3 
+ (d)  7.3 
+ 314  (a)  3.9 
+ (b)  11.1, 3.6 
+ (c) (1)  11.1 
+ (c) (2)  11.1 
+ (c) (3)  11.1 
+ (d)  11.1 
+ (e)  11.1 
+ (f)  N.A. 
+ 315  (a)  6.1(b) 
+ (b)  6.5 
+ (c)  6.1(a) 
+ (d)  6.1(c) 
+ (e)  5.13 
+ 316  (a) (1) (A)  5.11 
+ (a) (1) (B)  5.12 
+ (a) (2)  N.A. 
+ (b)  5.7 
+ (c)  5.6(b) 
+ 317  (a) (1)  5.3(b) 
+ (a) (2)  5.3(d) 
+ (b)  3.3 
+ 318  (a)  11.7 
+ 1  Note: This Cross Reference T able shall not, for  any purpose, be deemed to be part of this Indenture. 
+ 2  N.A. means Not Applicable. 
+ COPAR 2023-1 Indentur e 
+--- [START OF PAGE 3] ---
+ Page 
+ ARTICLE I  DEFINITIONS AND INCORPORA TION BY REFERENCE  2 
+ Section 1.1  Definitions  2 
+ Section 1.2  Incorporation by Reference of T rust Indenture Act  2 
+ Section 1.3  Other Interpretive Provisions  2 
+ ARTICLE II  THE NOTES  3 
+ Section 2.1  Form  3 
+ Section 2.2  Execution, Authentication and Delivery  3 
+ Section 2.3  Temporary Notes  4 
+ Section 2.4  Registration of T ransfer and Exchange  4 
+ Section 2.5  Mutilated, Destroyed, Lost or Stolen Notes  6 
+ Section 2.6  Persons Deemed Owners  6 
+ Section 2.7  Payment of Principal and Interest; Defaulted Interest  7 
+ Section 2.8  Cancellation  7 
+ Section 2.9  Release of Collateral  8 
+ Section 2.10  Book-Entry Notes  8 
+ Section 2.1 1  Notices to Clearing Agency  9 
+ Section 2.12  Definitive Notes  9 
+ Section 2.13  Authenticating Agents  10 
+ Section 2.14  Paying Agent  10 
+ Section 2.15  Tax and Accounting T reatment  11 
+ Section 2.16  Certain T ransfer Restrictions on all Classes of the Notes  11 
+ Section 2.17  Certain T ransfer Restrictions  12 
+ Section 2.18  Transfer Restrictions on Certain Notes Upon a Sale of a Certificate  12 
+ Section 2.19  Certain T ransfer Restrictions on the 144A Notes  13 
+ ARTICLE III  COVENANTS  17 
+ Section 3.1  Payment of Principal and Interest  17 
+ Section 3.2  Maintenance of Of fice or Agency  17 
+ Section 3.3  Money for Payments to Be Held in T rust  17 
+ Section 3.4  Existence  19 
+ Section 3.5  Protection of Collateral  19 
+--- [START OF PAGE 4] ---
+--- [START OF PAGE 5] ---
+ Page 
+ Section 3.6  Opinions as to Collateral  20 
+ Section 3.7  Performance of Obligations; Servicing of Receivables  20 
+ Section 3.8  Negative Covenants  21 
+ Section 3.9  Annual Compliance Statement  22 
+ Section 3.10  Restrictions on Certain Other Activities  23 
+ Section 3.1 1  Restricted Payments  23 
+ Section 3.12  Notice of Events of Default  23 
+ Section 3.13  Further Instruments and Acts  23 
+ Section 3.14  Compliance with Laws  23 
+ Section 3.15  Removal of Administrator  23 
+ Section 3.16  Perfection Representations, W arranties and Covenants  24 
+ Section 3.17  Investment Company Act Representation  24 
+ ARTICLE IV  SATISF ACTION AND DISCHARGE  24 
+ Section 4.1  Satisfaction and Dischar ge of Indenture  24 
+ Section 4.2  Application of T rust Money  25 
+ Section 4.3  Repayment of Monies Held by Paying Agent  25 
+ ARTICLE V  REMEDIES  25 
+ Section 5.1  Events of Default  25 
+ Section 5.2  Acceleration of Maturity; W aiver of Event of Default  26 
+ Section 5.3  Collection of Indebtedness and Suits for Enforcement by the Indenture T rustee  27 
+ Section 5.4  Remedies; Priorities  29 
+ Section 5.5  Optional Preservation of the Collateral  32 
+ Section 5.6  Limitation of Suits  32 
+ Section 5.7  Rights of Noteholders to Receive Principal and Interest  33 
+ Section 5.8  Restoration of Rights and Remedies  33 
+ Section 5.9  Rights and Remedies Cumulative  33 
+ Section 5.10  Delay or Omission Not a W aiver  33 
+ Section 5.1 1  Control by Noteholders  34 
+ Section 5.12  Waiver of Past Defaults  34 
+ Section 5.13  Undertaking for Costs  35 
+--- [START OF PAGE 6] ---
+--- [START OF PAGE 7] ---
+ Page 
+ Section 5.14  Waiver of Stay or Extension Laws  35 
+ Section 5.15  Action on Notes  35 
+ Section 5.16  Performance and Enforcement of Certain Obligations  35 
+ Section 5.17  Sale of Collateral  36 
+ ARTICLE VI  THE INDENTURE TRUSTEE  37 
+ Section 6.1  Duties of the Indenture T rustee  37 
+ Section 6.2  Rights of the Indenture T rustee  38 
+ Section 6.3  Individual Rights of the Indenture T rustee  40 
+ Section 6.4  The Indenture T rustee’ s Disclaimer  40 
+ Section 6.5  Notice of Defaults  40 
+ Section 6.6  Reports by the Paying Agent  40 
+ Section 6.7  Compensation and Indemnity  40 
+ Section 6.8  Removal, Resignation and Replacement of the Indenture T rustee  41 
+ Section 6.9  Successor Indenture T rustee by Mer ger  42 
+ Section 6.10  Appointment of Co-Indenture T rustee or Separate Indenture T rustee  43 
+ Section 6.1 1  Eligibility; Disqualification  44 
+ Section 6.12  Preferential Collection of Claims Against the Issuer  44 
+ Section 6.13  Representations and W arranties  44 
+ ARTICLE VII  NOTEHOLDERS’ LISTS AND REPOR TS  45 
+ Section 7.1  The Issuer to Furnish the Indenture T rustee Names and Addresses of Noteholders  45 
+ Section 7.2  Preservation of Information; Communications to Noteholders  45 
+ Section 7.3  Reports by the Indenture T rustee  45 
+ Section 7.4  Statements to Certificateholders and Noteholders  45 
+ Section 7.5  Noteholder Demand for Repurchase, Dispute Resolution  47 
+ Section 7.6  Investor Action to Initiate an Asset Review  48 
+ ARTICLE VIII  ACCOUNTS, DISBURSEMENTS AND RELEASES  49 
+ Section 8.1  Collection of Money  49 
+ Section 8.2  Trust Accounts  49 
+--- [START OF PAGE 8] ---
+ Page 
+ Section 8.3  General Provisions Regarding Accounts  51 
+ Section 8.4  Additional W ithdrawals and Deposits  54 
+ Section 8.5  Distributions  54 
+ Section 8.6  Release of Collateral  56 
+ Section 8.7  Opinion of Counsel  56 
+ ARTICLE IX  SUPPLEMENT AL INDENTURES  57 
+ Section 9.1  Supplemental Indentures W ithout Consent of Noteholders  57 
+ Section 9.2  Supplemental Indentures with Consent of Noteholders  58 
+ Section 9.3  Execution of Supplemental Indentures  59 
+ Section 9.4  Effect of Supplemental Indenture  60 
+ Section 9.5  Conformity with T rust Indenture Act  60 
+ Section 9.6  Reference in Notes to Supplemental Indentures  60 
+ ARTICLE X  REDEMPTION OF NOTES  60 
+ Section 10.1  Redemption  60 
+ Section 10.2  Form of Redemption Notice  61 
+ Section 10.3  Notes Payable on Redemption Date  61 
+ ARTICLE XI  MISCELLANEOUS  62 
+ Section 1 1.1  Compliance Certificates and Opinions, etc.  62 
+ Section 1 1.2  Form of Documents Delivered to the Indenture T rustee  63 
+ Section 1 1.3  Acts of Noteholders  64 
+ Section 1 1.4  Notices  65 
+ Section 1 1.5  Notices to Noteholders; W aiver  65 
+ Section 1 1.6  Alternate Payment and Notice Provisions  65 
+ Section 1 1.7  Conflict with T rust Indenture Act  65 
+ Section 1 1.8  Information Requests  66 
+ Section 1 1.9  Effect of Headings and T able of Contents  66 
+ Section 1 1.10  Successors and Assigns  66 
+ Section 1 1.11  Separability  66 
+ Section 1 1.12  Benefits of Indenture  66 
+ Section 1 1.13  Legal Holidays  66 
+--- [START OF PAGE 9] ---
+--- [START OF PAGE 10] ---
+ Page 
+ Section 1 1.14  GOVERNING LA W  66 
+ Section 1 1.15  Counterparts  66 
+ Section 1 1.16  Recording of Indenture  67 
+ Section 1 1.17  Trust Obligation  67 
+ Section 1 1.18  No Petition  67 
+ Section 1 1.19  Submission to Jurisdiction; W aiver of Jury T rial  68 
+ Section 1 1.20  Subordination of Claims  68 
+ Section 1 1.21  U.S.A Patriot Act  69 
+ Section 1 1.22  Beneficial Ownership  69 
+ Section 1 1.23  Limitation of Liability  69 
+ ARTICLE XII  COMPLIANCE WITH THE FDIC RULE  70 
+ Section 12.1  Purpose  70 
+ Section 12.2  Requirements of the FDIC Rule  71 
+ Section 12.3  Performance  72 
+ Section 12.4  Actions Upon Repudiation  73 
+ Section 12.5  Notice  75 
+ Section 12.6  Reservation of Rights  75 
+ Schedule I  Perfection Representations, W arranties and Covenants 
+ Exhibit A  Form of Notes 
+--- [START OF PAGE 11] ---
+ This INDENTURE, dated as of February 28, 2023 (as amended, supplemented, or otherwise modified and in ef fect from time to time, this 
+ “  Indenture  ”), is between CAPIT AL ONE PRIME AUT O RECEIV ABLES  TRUST 2023-1, a Delaware statutory trust (the “  Issuer  ”),  and W ilmington 
+ Trust, National Association, a national banking association, solely as trustee and not in its individual capacity (the “  Indenture T rustee  ”). 
+ Each party agrees as follows for the benefit of the other party and the equal and ratable benefit of the Holders of the Issuer ’s Class A-1 
+ 4.900% Auto Loan Asset Backed Notes (the “  Class A-1  Notes  ”), Class A-2 5.20% Auto Loan Asset Backed Notes  (the “  Class A-2 Notes  ”), Class 
+ A-3 4.87% Auto Loan Asset Backed Notes (the “  Class  A-3 Notes  ”), Class A-4 4.76% Auto Loan Asset Backed  Notes (the “  Class A-4 Notes  ”, and 
+ together with the Class A-1 Notes, the Class A-2 Notes and the Class A-3 Notes, the “  Class A Notes  ”), Class  B 5.07% Auto Loan Asset Backed 
+ Notes (the “  Class B Notes  ”), Class C 5.36% Auto Loan  Asset Backed Notes (the “  Class C Notes  ”) and Class  D 6.34% Auto Loan Asset Backed 
+ Notes (the “  Class D Notes  ”, and together with the  Class A-1 Notes, the Class A-2 Notes, the Class A-3 Notes, the Class A-4 Notes, the Class B Notes 
+ and the Class C Notes, the “  Notes  ”). 
+ GRANTING CLAUSE 
+ The Issuer , to secure the payment of principal of and interest on, and any other amounts owing in respect of, the Notes equally and ratably 
+ without prejudice, priority or distinction except as set forth herein, and to secure compliance with the provisions of this Indenture, hereby Grants in trust 
+ to the Indenture T rustee on the Closing Date, as trustee for the benefit of the Noteholders, all of the Issuer ’s right, title and interest, whether now owned 
+ or hereafter acquired, in and to (i) the T rust Estate and (ii) all present and future claims, demands, causes and choses in action in respect of any or all of 
+ the T rust Estate and all payments on or under and all proceeds of every kind and nature whatsoever in respect of any or all of the T rust Estate, including 
+ all proceeds of the conversion, voluntary or involuntary , into cash or other liquid property , all cash proceeds, accounts, accounts receivable, notes, drafts, 
+ acceptances, chattel paper , checks, deposit accounts, insurance proceeds, condemnation awards, rights to payment of any and every kind and other forms 
+ of obligations and receivables, instruments, securities, financial assets and other property which at any time constitute all or part of or are included in the 
+ proceeds of any of the T rust Estate (collectively , the “  Collateral  ”). 
+ The Indenture T rustee, on behalf of the Noteholders, acknowledges the foregoing Grant, accepts the trusts under this Indenture and 
+ agrees to perform its duties required in this Indenture in accordance with the provisions of this Indenture. 
+ The foregoing Grant is made in trust to secure (i) the payment of principal of and interest on, and any other amounts owing in respect of, 
+ the Notes, equally and ratably without prejudice, priority or distinction except as set forth herein and (ii) compliance with the provisions of this 
+ Indenture, all as provided in this Indenture. 
+ Without limiting the foregoing Grant, any Receivable repurchased or purchased by (a) the Servicer pursuant to  Section 3.6  of the Servicing 
+ Agreement or (b) by the Bank pursuant to  Section 3.4  of the Purchase Agreement shall be deemed to be automatically released from the lien of this 
+ Indenture without any action being taken by the Indenture T rustee upon payment by the applicable purchaser of the related Repurchase Price for such 
+ Repurchased Receivable. 
+ COPAR 2023-1 Indentur e 
+--- [START OF PAGE 12] ---
+ ARTICLE I 
+ DEFINITIONS AND INCORPORA TION BY REFERENCE 
+ SECTION 1.1  Definitions  . Capitalized terms are used  in this Indenture as defined in  A  p  p  endix A  to the  Sale Agreement, dated as of the 
+ date hereof (as amended, supplemented, or otherwise modified and in ef fect from time to time, the “  Sale  Agreement  ”), between the Issuer and Capital 
+ One Auto Receivables, LLC, which also contains rules as to usage that are applicable herein. 
+ SECTION 1.2  Incorporation by Reference of T rust Indenture  Act  . Whenever this Indenture refers to a provision  of the TIA, the provision 
+ is incorporated by reference in and made a part of this Indenture. The following TIA terms used in this Indenture have the following meanings: 
+ “  Commission  ” means the Securities and Exchange Commission. 
+ “  indenture securities  ” means the Notes. 
+ “  indenture securi  ty  holder  ” means a Noteholder . 
+ “  indenture to be qualified  ” means this Indenture. 
+ “  indenture trustee  ” or “  institutional trustee  ” means  the Indenture T rustee. 
+ “  obl  ig  or  ” on the indenture securities means the Issuer  and any other obligor on the indenture securities. 
+ All other TIA terms used in this Indenture that are defined by the TIA, defined by TIA reference to another statute or defined by 
+ Commission rule have the meaning assigned to them by such definitions. 
+ SECTION 1.3  Other Interpretive Provisions  . All terms  defined in this Indenture shall have the defined meanings when used in any 
+ certificate or other document delivered pursuant hereto unless otherwise defined therein. For purposes of this Indenture and all such certificates and 
+ other documents, unless the context otherwise requires: (a) accounting terms not otherwise defined in this Indenture, and accounting terms partly 
+ defined in this Indenture to the extent not defined, shall have the respective meanings given to them under GAAP (  provided  , that, to the extent that the 
+ definitions in this Indenture and GAAP conflict, the definitions in this Indenture shall control); (b) terms defined in Article 9 of the UCC as in ef fect in 
+ the relevant jurisdiction and not otherwise defined in this Indenture are used as defined in that Article; (c) the words “hereof,” “herein” and “hereunder” 
+ and words of similar import refer to this Indenture as a whole and not to any particular provision of this Indenture; (d) references to any Article, 
+ Section, Schedule, Appendix or Exhibit are references to Articles, Sections, Schedules, Appendices and Exhibits in or to this Indenture and references 
+ to any paragraph, subsection, clause or other subdivision within any Section or definition refer to such paragraph, subsection, clause or other 
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 11",
+      "error": "The term \"Holders\" is capitalized but not explicitly defined. While \"Noteholders\" is used frequently and its meaning is implied through cross-references to the TIA, inconsistent capitalization without a clear definition can lead to ambiguity.",
+      "suggestion": "Either define \"Holders\" or consistently use \"Noteholders\" (assuming \"Noteholders\" is a defined term in the Sale Agreement as per Section 1.1).",
+      "exact_quote": "the Holders of the Issuer’s Class A-1"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The verb \"Grants\" is capitalized as if it were a defined term, but it is used grammatically as an action verb.",
+      "suggestion": "Decapitalize \"Grants\" to \"grants\" unless it is specifically intended to be a defined legal term, in which case it should be explicitly defined and used consistently (e.g., \"makes a Grant\").",
+      "exact_quote": "hereby Grants in trust"
+    },
+    {
+      "location": "Page 12, Section 1.3",
+      "error": "The last sentence of Section 1.3 ends abruptly and is incomplete.",
+      "suggestion": "Complete the sentence or remove the incomplete phrase \"clause or other\" to ensure proper grammar and meaning.",
+      "exact_quote": "clause or other"
+    },
+    {
+      "location": "Page 12",
+      "error": "The footer on this page (internal page 2 of the document, as per the Table of Contents) is missing its page number.",
+      "suggestion": "Add the internal page number '2' to the footer of this page, consistent with the Table of Contents and standard document formatting.",
+      "exact_quote": "COPAR 2023-1 Indentur e"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-30 00:55:13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+EX-10 2 tmb-20250626xex10.htm EX-10
+FIRST AMENDMENT TO AMENDED AND RESTATED CREDIT
+AGREEMENT
+FIRST AMENDMENT TO AMENDED AND RESTATED CREDIT AGREEMENT
+(this “Agreement”), dated as of June 26, 2025 (and effective as set forth below), among
+MAYVILLE ENGINEERING COMPANY, INC., a Wisconsin corporation (the “Borrower”),
+the Subsidiary Guarantors (as defined in the Existing Credit Agreement referred to below)
+party hereto, the Incremental Lenders (as defined below), the Lenders (as defined below)
+party hereto (the “Consenting Lenders”), and WELLS FARGO BANK, NATIONAL
+ASSOCIATION, as administrative agent (the “Administrative Agent”). Unless otherwise
+indicated, all capitalized terms used herein and not otherwise defined herein shall have the
+respective meanings provided such terms in the Credit Agreement referred to below.
+W I T N E S S E T H:
+WHEREAS, the Borrower, the lenders party thereto (the “Lenders”) and the
+Administrative Agent have entered into that certain Amended and Restated Credit Agreement,
+dated as of June 28, 2023 (as amended, restated, supplemented or otherwise modified prior to
+the date hereof, the “Existing Credit Agreement” and as hereby amended and as from time to
+time further amended, modified, supplemented, restated, or amended and restated, the “Credit
+Agreement”);
+WHEREAS, the Borrower has requested an Incremental Revolving Credit Increase in
+the aggregate principal amount of $100,000,000, in accordance with Section 5.13 of the
+Existing Credit Agreement (the “First Amendment Revolving Credit Increase”);
+WHEREAS, subject to the terms of this Agreement, certain of the Revolving Credit
+Lenders identified on the signature pages hereto (each an “Incremental Lender”) are severally
+willing to provide a portion of the First Amendment Revolving Credit Increase; and
+WHEREAS, the Borrower has also requested, and subject to the terms and conditions
+set forth herein, the Administrative Agent and the Consenting Lenders have agreed to further
+amend the Existing Credit Agreement as more specifically set forth herein.
+NOW, THEREFORE, in consideration of the foregoing and for other good and
+valuable consideration, the receipt and sufficiency of which are hereby acknowledged, it is
+agreed as follows:
+SECTION 1.Amendments to Existing Credit Agreement. Effective as of the First
+Amendment Effective Date (as defined below) and subject to the terms and conditions set
+forth herein and in reliance upon the representations and warranties set forth herein:
+(a)Schedule 1.1 (Commitments and Commitment Percentages) to the Existing
+Credit Agreement is hereby amended and restated in the form attached hereto
+as Annex A.
+(b)the body of Existing Credit Agreement is hereby amended as follows: (i) to
+delete red or green stricken text (indicated textually in the same manner as the
+following examples: stricken text and stricken text) and (ii) to add the blue or
+green double-underlined text (indicated textually in the same manner as the
+following examples: double-underlined text and double-underlined text), in
+each case, as set forth in the conformed copy attached hereto as Annex B.
+--- [START OF PAGE 2] ---
+1
+--- [START OF PAGE 3] ---
+SECTION 2.Revolving Credit Facility Increase; Reallocation.
+(a)Each Incremental Lender severally agrees that its Revolving Credit
+Commitment after giving effect to the First Amendment Revolving Credit
+Increase shall be as set forth opposite such Lender’s name on Annex A hereto.
+(b)The parties hereto hereby agree that (i) this Agreement constitutes a request
+for an Incremental Revolving Credit Increase pursuant to Section 5.13 of the
+Credit Agreement, (ii) the parties hereto hereby waive any prior notice
+required thereby, and (iii) this Agreement shall be deemed to be an “Lender
+Joinder Agreement” in accordance with Section 5.13(h) of the Credit
+Agreement.
+(c)Pursuant to Section 5.13 of the Credit Agreement, on the First Amendment
+Effective Date (as defined below) and after giving effect to this Agreement,
+the outstanding Revolving Credit Loans and Revolving Credit Commitment
+Percentages of Swingline Loans and L/C Obligations will be reallocated by
+the Administrative Agent among the Revolving Credit Lenders (including the
+Incremental Lenders providing the First Amendment Revolving Credit
+Increase) in accordance with their revised Revolving Credit Commitment
+Percentages (and the Revolving Credit Lenders (including the Incremental
+Lenders providing the First Amendment Revolving Credit Increase) agree to
+make all payments and adjustments necessary to effect such reallocation and
+the Borrower shall pay any and all costs required pursuant to Section 5.9 of
+the Credit Agreement in connection with such reallocation as if such
+reallocation were a repayment).
+SECTION 3.Conditions of Effectiveness of this Agreement.  This Agreement shall
+become effective on the date when the following conditions shall have been satisfied or
+waived (such date, the “First Amendment Effective Date”):
+(a) The Administrative Agent’s receipt of the following, each in form and
+substance reasonably satisfactory to the Administrative Agent:
+(i) this Agreement, duly executed by each of the Credit Parties existing
+as of the First Amendment Effective Date, the Administrative Agent, each
+Incremental Lender and each of the Consenting Lenders;
+(ii) a certificate of a Responsible Officer (or the secretary or assistant
+secretary) of each Credit Party certifying as to the incumbency and genuineness of the
+signature of each officer of such Credit Party executing Loan Documents to which it
+is a party and certifying that attached thereto is a true, correct and complete copy of
+(A) the articles or certificate of incorporation or formation (or equivalent), as
+applicable, of such Credit Party and all amendments thereto, certified as of a recent
+date by the appropriate Governmental Authority in its jurisdiction of incorporation,
+organization or formation (or equivalent), as applicable, (B) the bylaws or other
+governing document of such Credit Party as in effect on the First Amendment
+Effective Date, (C) resolutions duly adopted by the board of directors (or other
+governing body) of such Credit Party authorizing and approving the transactions
+contemplated hereunder and the execution, delivery and performance of this
+Amendment, the Credit Agreement and the other Loan Documents to which it is a
+party, and (D) certificates as of a recent date of the good standing of each Credit Party
+--- [START OF PAGE 4] ---
+2under the laws of its jurisdiction of incorporation, organization or formation (or
+equivalent), as applicable;
+(iii) an Officer’s Compliance Certificate demonstrating, in form and
+substance reasonably satisfactory to the Administrative Agent, that the Borrower is in
+compliance with the
+--- [START OF PAGE 5] ---
+financial covenants set forth in Section 9.15 of the Credit Agreement as of the First
+Amendment Effective Date based on the financial statements most recently delivered
+pursuant to Section 8.1(a) or 8.1(b) of the Existing Credit Agreement, as applicable,
+both before and after giving effect (on a pro forma basis) to (x) any Incremental
+Revolving Credit Commitment, and (y) the making of the First Amendment
+Revolving Credit Increase pursuant thereto (with such Incremental Revolving Credit
+Commitment being deemed to be fully funded);
+(iv) a certificate from the chief financial officer of the Borrower with
+respect to solvency (on a consolidated basis) of the Borrower and its Subsidiaries as
+of the First Amendment Effective Date after giving effect to the First Amendment
+Revolving Credit Increase and the other amendments contemplated by this
+Agreement;
+(v) an opinion from counsel to the Credit Parties, in form and substance
+reasonably satisfactory to the Administrative Agent.
+(b) The representations and warranties set forth in Section 3 shall be true and
+correct.
+(c) No Default or Event of Default shall exist on the First Amendment Effective
+Date immediately prior to or after giving effect to this Agreement.
+(d) The Administrative Agent shall have received the results of a Lien search, in
+form and substance reasonably satisfactory thereto, made against the Credit Parties under the
+Uniform Commercial Code (or applicable judicial docket) as in effect in each jurisdiction in
+which filings or recordations under the Uniform Commercial Code should be made to
+evidence or perfect security interests in all assets of such Credit Party, indicating among other
+things that the assets of each such Credit Party are free and clear of any Lien (except for
+Permitted Liens).
+(e) All governmental, shareholder and third party consents and approvals
+necessary (or any other material consents as determined in the reasonable discretion of the
+Administrative Agent) in connection with the transactions contemplated by this Agreement
+shall have been obtained and shall be in full force and effect.
+(f) The Borrower and each of the Subsidiary Guarantors shall have provided to
+the Administrative Agent and the Lenders, at least five (5) Business Days prior to the First
+Amendment Effective Date, a Beneficial Ownership Certification under 31 C.F.R. 1010.230
+and all documentation and other information required by regulatory authorities under
+applicable “know your customer”, anti-money-laundering, beneficial ownership and other
+similar rules and regulations, including, without limitation, the PATRIOT Act.
+(g) The Borrower shall have paid all fees and expenses required to be paid on the
+First Amendment Effective Date.
+For purposes of determining compliance with the conditions specified in this Section 3, the
+Administrative Agent, each Incremental Lender and each Consenting Lender that has signed
+this Agreement shall be deemed to have consented to, approved or accepted or to be satisfied
+with, each document or other matter required thereunder to be consented to or approved by or
+acceptable or satisfactory to an Incremental Lender and/or a Consenting Lender, as applicable,
+unless the Administrative Agent shall have received notice from such Incremental Lender
+--- [START OF PAGE 6] ---
+3and/or Consenting Lender, as applicable, prior to the proposed First Amendment Effective
+Date specifying its objection thereto.
+--- [START OF PAGE 7] ---
+SECTION 4.Representations and Warranties.  To induce the Administrative Agent,
+the Incremental Lenders party hereto and the Consenting Lenders party hereto to enter into
+this Agreement, each Credit Party represents and warrants to the Administrative Agent, the
+Incremental Lenders and the Consenting Lenders on and as of the First Amendment Effective
+Date that, in each case:
+(a) each of the representations and warranties contained in Article VII of the
+Credit Agreement are true and correct in all material respects, except to the extent any such
+representation and warranty is qualified by materiality or reference to Material Adverse
+Effect, in which case, such representation and warranty is true, correct and complete in all
+respects, with the same effect as if made on and as of such date (except for any such
+representation and warranty that by its terms is made only as of an earlier date, which
+representation and warranty remains true and correct as of such earlier date);
+(b) no Default or Event of Default has occurred and is continuing immediately
+prior to or after giving effect to this Agreement;
+(c) it has the right, power and authority and has taken all necessary corporate and
+other action to authorize the execution, delivery and performance of this Agreement in
+accordance with their respective terms; and
+(d) this Agreement has been duly executed and delivered by the duly authorized
+officers, managers, managing members or other authorized person of each Credit Party that is
+a party thereto, and each such document constitutes the legal, valid and binding obligation of
+each Credit Party, enforceable in accordance with its terms, except as such enforceability may
+be limited by bankruptcy, insolvency, reorganization, moratorium or similar state or federal
+Debtor Relief Laws from time to time in effect which affect the enforcement of creditors’
+rights in general and the availability of equitable remedies.
+SECTION 5.Credit Party Acknowledgements, Agreements and Confirmations.  By
+its execution of this Agreement, each Credit Party hereby (a) consents to this Agreement and
+agrees that the transactions contemplated by this Agreement shall not limit or diminish the
+obligations of such Credit Party, or release such Credit Party from any obligations, under any
+of the Loan Documents to which it is a party, (b) confirms and reaffirms its obligations under
+each of the Loan Documents to which it is a party and (c) agrees that each of the Loan
+Documents to which it is a party remain in full force and effect and are hereby ratified and
+confirmed.
+SECTION 6.Reference to and Effect on the Credit Agreement and the Loan
+Documents.
+(a) On and after the First Amendment Effective Date, each reference in the Credit
+Agreement to “this Agreement,” “herein,” “hereto”, “hereof” and “hereunder” or words of like
+import referring to the Credit Agreement, and each reference in the Notes and each of the
+other Loan Documents to “the Credit Agreement”, “thereunder”, “thereof” or words of like
+import referring to the Credit Agreement, shall mean and be a reference to the Credit
+Agreement, as amended and supplemented by this Agreement.
+(b) The Credit Agreement and each of the other Loan Documents, as specifically
+amended and supplemented by this Agreement, are and shall continue to be in full force and
+effect and are hereby in all respects ratified and confirmed.
+(c) The execution, delivery and effectiveness of this Agreement shall not, except
+as expressly provided herein, operate as a waiver of any right, power or remedy of any Lender
+or the Administrative Agent under any of the Loan Documents, nor constitute a waiver of any
+provision of any of the Loan Documents.  Without limiting the generality of the foregoing, the
+--- [START OF PAGE 8] ---
+4Security Documents in effect immediately prior to the date hereof and all of the Collateral
+described therein in existence immediately prior to the date hereof do and shall continue to
+secure the payment of all Secured Obligations.  
+--- [START OF PAGE 9] ---
+5(d) This Agreement is the entire agreement, and supersedes any prior agreements
+and contemporaneous oral agreements, of the parties concerning its subject matter. This
+Agreement shall constitute a “Loan Document” for all purposes of the Credit Agreement and
+the other Loan Documents.
+(e) This Agreement shall be binding on and inure to the benefit of the parties
+hereto and their successors and permitted assigns.
+SECTION 7.Costs and Expenses.  The Borrower hereby reconfirms its obligations
+pursuant to Section 12.3 of the Credit Agreement to pay and reimburse the Administrative
+Agent for all reasonable fees, costs and expenses in accordance with the terms thereof.
+SECTION 8.Governing Law; Jury Trial Waiver.  This Agreement and any claim,
+controversy, dispute or cause of action (whether in contract or tort or otherwise) based upon,
+arising out of or relating to this Agreement and the transactions contemplated hereby shall be
+governed by, and construed in accordance with, the law of the State of New York.  EACH
+PARTY HERETO HEREBY IRREVOCABLY WAIVES, TO THE FULLEST EXTENT
+PERMITTED BY APPLICABLE LAW, ANY RIGHT IT MAY HAVE TO A TRIAL BY JURY
+IN ANY LEGAL PROCEEDING DIRECTLY OR INDIRECTLY ARISING OUT OF OR
+RELATING TO THIS AGREEMENT OR THE TRANSACTIONS CONTEMPLATED
+HEREBY (WHETHER BASED ON CONTRACT, TORT OR ANY OTHER THEORY).  EACH
+PARTY HERETO (A) CERTIFIES THAT NO REPRESENTATIVE, AGENT OR ATTORNEY
+OF ANY OTHER PERSON HAS REPRESENTED, EXPRESSLY OR OTHERWISE, THAT
+SUCH OTHER PERSON WOULD NOT, IN THE EVENT OF LITIGATION, SEEK TO
+ENFORCE THE FOREGOING WAIVER AND (B) ACKNOWLEDGES THAT IT AND THE
+OTHER PARTIES HERETO HAVE BEEN INDUCED TO ENTER INTO THIS AGREEMENT
+BY, AMONG OTHER THINGS, THE MUTUAL WAIVERS AND CERTIFICATIONS IN THIS
+SECTION.
+SECTION 9.Counterparts; Electronic Execution. This Agreement may be executed
+in counterparts (and by different parties hereto in different counterparts), each of which shall
+constitute an original, but all of which when taken together shall constitute a single contract.
+Delivery of an executed counterpart of a signature page of this Agreement by facsimile or in
+electronic (i.e., “pdf” or “tif”) format shall be effective as delivery of a manually executed
+counterpart of this Agreement. This Agreement may be executed by Electronic Signatures or
+in the form of an Electronic Record pursuant to, and in accordance with, the provisions of
+Section 12.16 of the Credit Agreement.
+[Signature pages to follow]
+--- [START OF PAGE 10] ---
+Mayville Engineering Company, Inc.IN WITNESS WHEREOF, the parties hereto have caused their duly authorized
+officers to execute and deliver this Agreement as of the date first above written.
+BORROWER:
+MAYVILLE ENGINEERING COMPANY,
+INC.
+SUBSIDIARY GUARANTORS:
+CENTER MANUFACTURING
+HOLDINGS, INC.
+CENTER MANUFACTURING, INC.
+CENTER – MOELLER PRODUCTS LLC
+DEFIANCE METAL PRODUCTS CO.
+DEFIANCE METAL PRODUCTS OF
+ARKANSAS, INC. 
+ By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+By:
+Name:
+Title:
+--- [START OF PAGE 11] ---
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature Page
+--- [START OF PAGE 12] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageDEFIANCE METAL PRODUCTS OF PA.,
+INC.
+MID-STATES ALUMINUM, LLC 
+ By:
+Name:
+Title:
+By:
+Name:
+Title:
+--- [START OF PAGE 13] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageWELLS FARGO BANK, NATIONAL
+ASSOCIATION, as Administrative Agent,
+Issuing Lender, Swingline Lender,
+Consenting Lender and an Incremental
+Lender
+By:
+___________________________________
+Name:
+Title:  
+--- [START OF PAGE 14] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageJPMORGAN CHASE BANK, N.A., as a
+Consenting Lender and an Incremental
+Lender
+By:
+___________________________________
+Name:
+Title:  
+--- [START OF PAGE 15] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageTD BANK, N.A., as a Consenting Lender
+and an Incremental Lender
+By:
+___________________________________
+Name:
+Title:  
+--- [START OF PAGE 16] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageCITIBANK, N.A., as a Consenting Lender
+By:
+___________________________________
+Name:
+Title:  
+--- [START OF PAGE 17] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageHANMI BANK, as a Consenting Lender and
+an Incremental Lender
+By:
+___________________________________
+Name:
+Title:  
+--- [START OF PAGE 18] ---
+Mayville Engineering Company, Inc.
+First Amendment to A&amp;R Credit Agreement (Revolver Increase)
+Signature PageASSOCIATED BANK, N.A., as a
+Consenting Lender and an Incremental
+Lender
+By:
+___________________________________
+Name:
+Title:  
+--- [START OF PAGE 19] ---
+Annex A
+REVOLVING CREDIT COMMITMENTS AND REVOLVING CREDIT COMMITMENT
+PERCENTAGES
+Lender Revolving
+Credit
+CommitmentRevolving
+Credit
+Commitment
+Percentage
+Wells Fargo Bank, National
+Association 
+$108,000,000.00 30.857142858%
+JPMorgan Chase Bank, N.A.  $90,000,000.00 25.714285714%
+TD Bank, N.A.  $77,000,000.00 22.000000000%
+Associated Bank, N.A.  $30,000,000.00 8.571428571%
+Hanmi Bank  $25,000,000.00 7.142857143%
+Citibank, N.A.  $20,000,000.00 5.714285714%
+Total $350,000,000.00100.000000000%
+--- [START OF PAGE 20] ---
+ANNEX B
+Published CUSIP Number: 57859VAP8
+$350,000,000.00
+AMENDED AND RESTATED CREDIT AGREEMENT
+dated as of June 28, 2023
+(as amended by that certain First Amendment to Amended and Restated Credit Agreement
+dated as of June 26, 2025)
+by and among
+MAYVILLE ENGINEERING COMPANY, INC.
+as Borrower,
+the Lenders referred to herein,
+as Lenders,
+and
+WELLS FARGO BANK, NATIONAL ASSOCIATION,
+as Administrative Agent,
+Swingline Lender and Issuing Lender
+and
+WELLS FARGO SECURITIES, LLC,
+as Joint Lead Arranger and Joint Bookrunner
+and
+J.P. MORGAN SECURITIES LLC,
+as Joint Lead Arranger and Joint Bookrunner
+and
+TD BANK, N.A.,
+as Joint Lead Arranger and Joint Bookrunner 
+--- [START OF PAGE 21] ---
+--- [START OF PAGE 22] ---
+i 
+ ARTICLE IDEFINITIONS 1
+SECTION 1.1Definitions 1
+SECTION 1.2Other Definitions and Provisions 31
+SECTION 1.3Accounting Terms 31
+SECTION 1.4UCC Terms 32
+SECTION 1.5Rounding 32
+SECTION 1.6References to Agreement and Laws 32
+SECTION 1.7Times of Day 32
+SECTION 1.8Letter of Credit Amounts 32
+SECTION 1.9Guarantees/Earn-Outs 33
+SECTION 1.10Covenant Compliance Generally 33
+SECTION 1.11Rates 33
+SECTION 1.12Divisions 33
+ARTICLE IIREVOLVING CREDIT FACILITY 34
+SECTION 2.1Revolving Credit Loans 34
+SECTION 2.2Swingline Loans 34
+SECTION 2.3Procedure for Advances of Revolving Credit Loans and Swingline
+Loans 36
+SECTION 2.4Repayment and Prepayment of Revolving Credit Loans and Swingline
+Loans 37
+SECTION 2.5Permanent Reduction of the Revolving Credit Commitment 37
+SECTION 2.6Termination of Revolving Credit Facility 38
+ARTICLE IIILETTER OF CREDIT FACILITY 38
+SECTION 3.1L/C Facility 38
+SECTION 3.2Procedure for Issuance of Letters of Credit 39
+SECTION 3.3Commissions and Other Charges 39
+SECTION 3.4L/C Participations 40
+SECTION 3.5Reimbursement Obligation of the Borrower 41
+SECTION 3.6Obligations Absolute 41
+SECTION 3.7Effect of Letter of Credit Application 41
+SECTION 3.8Resignation of Issuing Lenders 42
+SECTION 3.9Reporting of Letter of Credit Information and L/C Commitment 42
+SECTION 3.10Letters of Credit Issued for Subsidiaries 42
+--- [START OF PAGE 23] ---
+ii 
+ ARTICLE IVReserved 43
+ARTICLE VGENERAL LOAN PROVISIONS 43
+SECTION 5.1Interest 43
+SECTION 5.2Notice and Manner of Conversion or Continuation of Loans 44
+SECTION 5.3Fees 44
+SECTION 5.4Manner of Payment 45
+SECTION 5.5Evidence of Indebtedness 45
+SECTION 5.6Sharing of Payments by Lenders 46
+SECTION 5.7Administrative Agent’s Clawback 46
+SECTION 5.8Changed Circumstances 47
+SECTION 5.9Indemnity 50
+SECTION 5.10Increased Costs 50
+SECTION 5.11Taxes 51
+SECTION 5.12Mitigation Obligations; Replacement of Lenders 55
+SECTION 5.13Incremental Loans 56
+SECTION 5.14Cash Collateral 58
+SECTION 5.15Defaulting Lenders 58
+ARTICLE VICONDITIONS OF CLOSING AND BORROWING 60
+SECTION 6.1Conditions to Closing and Initial Extensions of Credit 60
+SECTION 6.2Conditions to All Extensions of Credit 64
+ARTICLE VIIREPRESENTATIONS AND WARRANTIES OF THE CREDIT PARTIES64
+SECTION 7.1Organization; Power; Qualification 64
+SECTION 7.2Ownership 65
+SECTION 7.3Authorization; Enforceability 65
+SECTION 7.4Compliance of Agreement, Loan Documents and Borrowing with
+Laws, Etc 65
+SECTION 7.5Compliance with Law; Governmental Approvals 65
+SECTION 7.6Tax Returns and Payments 66
+SECTION 7.7Intellectual Property Matters 66
+SECTION 7.8Environmental Matters 66
+SECTION 7.9Employee Benefit Matters 67
+SECTION 7.10Margin Stock 68
+SECTION 7.11Government Regulation 68
+SECTION 7.12Material Contracts 68
+SECTION 7.13Employee Relations 68
+--- [START OF PAGE 24] ---
+--- [START OF PAGE 25] ---
+iii 
+ SECTION 7.14Burdensome Provisions 69
+SECTION 7.15Financial Statements 69
+SECTION 7.16No Material Adverse Change 69
+SECTION 7.17Solvency 69
+SECTION 7.18Title to Properties 69
+SECTION 7.19Litigation 69
+SECTION 7.20Anti-Corruption Laws; Anti-Money Laundering Laws; Sanctions and
+Outbound Investment Rules 69
+SECTION 7.21Absence of Defaults 70
+SECTION 7.22ESOP 70
+SECTION 7.23Senior Indebtedness Status 71
+SECTION 7.24Disclosure 71
+ARTICLE VIIIAFFIRMATIVE COVENANTS 72
+SECTION 8.1Financial Statements and Budgets 72
+SECTION 8.2Certificates; Other Reports 73
+SECTION 8.3Notice of Litigation and Other Matters 73
+SECTION 8.4Preservation of Corporate Existence and Related Matters 75
+SECTION 8.5Maintenance of Property and Licenses 75
+SECTION 8.6Insurance 75
+SECTION 8.7Accounting Methods and Financial Records 76
+SECTION 8.8Payment of Taxes and Other Obligations 76
+SECTION 8.9Compliance with Laws and Approvals 76
+SECTION 8.10Environmental Laws 76
+SECTION 8.11Compliance with ERISA 76
+SECTION 8.12Compliance with Material Contracts 76
+SECTION 8.13Visits and Inspections 76
+SECTION 8.14Additional Subsidiaries 77
+SECTION 8.15Depository Bank 77
+SECTION 8.16Use of Proceeds 78
+SECTION 8.17ESOP 78
+SECTION 8.18Compliance with Anti-Corruption Laws; Beneficial Ownership
+Regulation, Anti-Money Laundering Laws and Sanctions 78
+SECTION 8.19Further Assurances 78
+SECTION 8.20Post-Closing Matters 79
+SECTION 8.21Lender Meetings 79
+--- [START OF PAGE 26] ---
+--- [START OF PAGE 27] ---
+iv 
+ ARTICLE IXNEGATIVE COVENANTS 79
+SECTION 9.1Indebtedness 79
+SECTION 9.2Liens 80
+SECTION 9.3Investments 81
+SECTION 9.4Fundamental Changes 82
+SECTION 9.5Asset Dispositions 83
+SECTION 9.6Restricted Payments 84
+SECTION 9.7Transactions with Affiliates 84
+SECTION 9.8Accounting Changes; Organizational Documents 84
+SECTION 9.9Payments and Modifications of Subordinated Indebtedness 85
+SECTION 9.10No Further Negative Pledges; Restrictive Agreements 85
+SECTION 9.11ESOP Matters 86
+SECTION 9.12Sale of Accounts 86
+SECTION 9.13Sale Leasebacks 86
+SECTION 9.14Capital Expenditures 86
+SECTION 9.15Financial Covenants 86
+SECTION 9.16No Amendment to ESOP Documentation 87
+SECTION 9.17Limitations Regarding Outbound Investment Rules 87
+ARTICLE XDEFAULT AND REMEDIES 87
+SECTION 10.1Events of Default 87
+SECTION 10.2Remedies 89
+SECTION 10.3Rights and Remedies Cumulative; Non-Waiver; etc 90
+SECTION 10.4Crediting of Payments and Proceeds 91
+SECTION 10.5Administrative Agent May File Proofs of Claim 91
+SECTION 10.6Credit Bidding 92
+ARTICLE XITHE ADMINISTRATIVE AGENT 92
+SECTION 11.1Appointment and Authority 92
+SECTION 11.2Rights as a Lender 93
+SECTION 11.3Exculpatory Provisions 93
+SECTION 11.4Reliance by the Administrative Agent 94
+SECTION 11.5Delegation of Duties 94
+SECTION 11.6Resignation of Administrative Agent 95
+SECTION 11.7Non-Reliance on Administrative Agent and Other Lenders 96
+SECTION 11.8No Other Duties, Etc 96
+SECTION 11.9Collateral and Guaranty Matters 96
+--- [START OF PAGE 28] ---
+--- [START OF PAGE 29] ---
+v 
+ SECTION 11.10Secured Hedge Agreements and Secured Cash Management
+Agreements 97
+SECTION 11.11[Reserved.] 97
+SECTION 11.12Erroneous Payments 97
+ARTICLE XIIMISCELLANEOUS 99
+SECTION 12.1Notices 99
+SECTION 12.2Amendments, Waivers and Consents 101
+SECTION 12.3Expenses; Indemnity 103
+SECTION 12.4Right of Setoff 105
+SECTION 12.5Governing Law; Jurisdiction, Etc 105
+SECTION 12.6Waiver of Jury Trial 106
+SECTION 12.7Reversal of Payments 106
+SECTION 12.8Injunctive Relief 107
+SECTION 12.9Successors and Assigns; Participations 107
+SECTION 12.10Treatment of Certain Information; Confidentiality 110
+SECTION 12.11Performance of Duties 111
+SECTION 12.12All Powers Coupled with Interest 111
+SECTION 12.13Survival 111
+SECTION 12.14Titles and Captions 112
+SECTION 12.15Severability of Provisions 112
+SECTION 12.16Counterparts; Integration; Effectiveness; Electronic Execution 112
+SECTION 12.17Term of Agreement 113
+SECTION 12.18USA PATRIOT Act; Anti-Money Laundering Laws 113
+SECTION 12.19Independent Effect of Covenants 113
+SECTION 12.20No Advisory or Fiduciary Responsibility 113
+SECTION 12.21Amendment and Restatement; No Novation 114
+SECTION 12.22Inconsistencies with Other Documents 115
+SECTION 12.23Acknowledgement and Consent to Bail-In of Affected Financial
+Institutions 115
+SECTION 12.24Certain ERISA Matters 115
+SECTION 12.25Acknowledgement Regarding Any Supported QFCs 116
+--- [START OF PAGE 30] ---
+viEXHIBITS
+Exhibit A-1 -Form of Revolving Credit Note
+Exhibit A-2 -Form of Swingline Note
+Exhibit B -Form of Notice of Borrowing
+Exhibit C -Form of Notice of Account Designation
+Exhibit D -Form of Notice of Prepayment
+Exhibit E -Form of Notice of Conversion/Continuation
+Exhibit F -Form of Officer’s Compliance Certificate
+Exhibit G -Form of Assignment and Assumption
+Exhibit H-1 -Form of U.S. Tax Compliance Certificate (Non-
+Partnership Foreign Lenders)
+Exhibit H-2 -Form of U.S. Tax Compliance Certificate (Non-
+Partnership Foreign Participants)
+Exhibit H-3 -Form of U.S. Tax Compliance Certificate (Foreign
+Participant Partnerships)
+Exhibit H-4 -Form of U.S. Tax Compliance Certificate (Foreign Lender
+Partnerships)
+Exhibit I -Form of Joinder Agreement
+SCHEDULES
+Schedule 1.1 -Commitments and Commitment Percentages
+Schedule 7.1 -Jurisdictions of Organization and Qualification
+Schedule 7.2 -Subsidiaries and Capitalization
+Schedule 7.6 -Tax Matters
+Schedule 7.9 -ERISA Plans
+Schedule 7.12 -Material Contracts
+Schedule 7.13 -Labor and Collective Bargaining Agreements
+Schedule 7.18 -Real Property
+Schedule 7.19 -Litigation
+Schedule 8.20 -Post-Closing Matters
+Schedule 9.1 -Existing Indebtedness
+Schedule 9.2 -Existing Liens
+Schedule 9.3 -Existing Loans, Advances and Investments
+Schedule 9.7 -Transactions with Affiliates
+Schedule 12.21 -Existing Letters of Credit
+--- [START OF PAGE 31] ---
+AMENDED AND RESTATED CREDIT AGREEMENT, dated as of June 28, 2023, by and
+among MAYVILLE ENGINEERING COMPANY, INC., a Wisconsin corporation (“Mayville” or the
+“Borrower”), the lenders who are party to this Agreement and the lenders who may become a party to
+this Agreement pursuant to the terms hereof, as Lenders, and WELLS FARGO BANK, NATIONAL
+ASSOCIATION, a national banking association, as Administrative Agent for the Lenders.
+STATEMENT OF PURPOSE
+The Borrower, the lenders party thereto, and WELLS FARGO BANK, NATIONAL
+ASSOCIATION, a national banking association, as administrative agent for such lenders, are party to
+that certain Amended and Restated Credit Agreement dated as of September 26, 2019 (as amended to
+date, the “Existing Credit Agreement”).  
+The Borrower has requested, and subject to the terms and conditions set forth in this
+Agreement, the Administrative Agent and the Lenders have agreed to extend certain credit facilities
+to the Borrower to be used, in part, to restructure, and to increase, the indebtedness and other
+obligations outstanding under the Existing Credit Agreement and amend and restate the Existing
+Credit Agreement in its entirety.
+NOW, THEREFORE, for good and valuable consideration, the receipt and sufficiency of
+which are hereby acknowledged by the parties hereto, such parties hereby agree as follows:
+ARTICLE I
+DEFINITIONS
+SECTION 1.1 Definitions.  The following terms when used in this Agreement shall
+have the meanings assigned to them below:
+“Accu-Fab Acquisition” means the contemplated Acquisition by the Borrower of all of the
+outstanding Equity Interests of Accu-Fab, LLC, a Delaware limited liability company, from Tide
+Rock Yieldco, LLC, a Delaware limited liability company, pursuant to that certain Purchase
+Agreement, dated as of May 23, 2025, by and among the Borrower, Accu-Fab, LLC and Tide Rock
+Yieldco, LLC.  
+“Acquisition” means any transaction, or any series of related transactions, consummated on
+or after the date of this Agreement, by which any Credit Party or any of its </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1(a)",
+      "error": "The capitalized term \"Amendment\" is used but not defined. The document defines \"this Agreement\" (capitalized) to refer to the First Amendment to Amended and Restated Credit Agreement, so \"Amendment\" should likely be \"Agreement\" for consistency.",
+      "suggestion": "Replace \"this Amendment\" with \"this Agreement\".",
+      "exact_quote": "delivery and performance of this Amendment"
+    },
+    {
+      "location": "Page 3, Section 3(a)(ii)",
+      "error": "The sentence ends abruptly and carries over to the next page without proper continuation, indicating a drafting error or forgotten placeholder.",
+      "suggestion": "Complete the sentence or ensure proper pagination and sentence flow.",
+      "exact_quote": "certificates as of a recent date of the good standing of each Credit Party"
+    },
+    {
+      "location": "Page 4, Section 3(a)(iii)",
+      "error": "The sentence ends abruptly and carries over to the next page without proper continuation, indicating a drafting error or forgotten placeholder.",
+      "suggestion": "Complete the sentence or ensure proper pagination and sentence flow.",
+      "exact_quote": "the Borrower is in compliance with the"
+    },
+    {
+      "location": "Page 5, Section 3(b)",
+      "error": "The condition refers to 'Section 3' for representations and warranties, but the representations and warranties are actually set forth in 'Section 4'. This appears to be a numbering error.",
+      "suggestion": "Change 'Section 3' to 'Section 4'.",
+      "exact_quote": "The representations and warranties set forth in Section 3 shall be true and correct."
+    },
+    {
+      "location": "Page 9",
+      "error": "A placeholder indicates that signature pages are expected to follow, which is a drafting error in a completed document.",
+      "suggestion": "Remove the placeholder or replace it with appropriate text if the document is finalized.",
+      "exact_quote": "[Signature pages to follow]"
+    },
+    {
+      "location": "Page 47, Article I (Definitions)",
+      "error": "There is a pagination error. The page number is '13', but it should sequentially be '14' after the preceding page (Page 46) which was '13'.",
+      "suggestion": "Correct the page number to '14'.",
+      "exact_quote": "13"
+    },
+    {
+      "location": "Page 49, Article I (Definitions)",
+      "error": "There is a pagination error. The page number is '14', but it should sequentially be '15' after the preceding page (Page 48) which was '14'.",
+      "suggestion": "Correct the page number to '15'.",
+      "exact_quote": "14"
+    },
+    {
+      "location": "Page 54, Article I (Definitions)",
+      "error": "The singular term 'Note' is capitalized and used in the definition of 'Loan Documents' but is not explicitly defined. While 'Notes' (plural) is defined later, consistency requires either 'Note' to be defined or 'Notes' to be used consistently.",
+      "suggestion": "Define 'Note' as the singular of 'Notes' or replace 'each Note' with 'the Notes' in the definition of 'Loan Documents'.",
+      "exact_quote": "each Note"
+    },
+    {
+      "location": "Page 55, Article I (Definitions)",
+      "error": "The capitalized term 'Outstanding Amount' is used in the definition of 'Minimum Collateral Amount' but is not defined.",
+      "suggestion": "Add a definition for 'Outstanding Amount'.",
+      "exact_quote": "Outstanding Amount"
+    },
+    {
+      "location": "Page 60, Article I (Definitions)",
+      "error": "There is a typographical error in 'Sanctioned Peron(s)'. It should be 'Sanctioned Person(s)'.",
+      "suggestion": "Correct 'Peron(s)' to 'Person(s)'.",
+      "exact_quote": "Sanctioned Peron(s)"
+    },
+    {
+      "location": "Page 63, Article I (Definitions)",
+      "error": "The phrase 'for the ratable benefit and the Secured Parties' contains a grammatical error. It should likely be 'for the ratable benefit of the Secured Parties'.",
+      "suggestion": "Change 'benefit and the Secured Parties' to 'benefit of the Secured Parties'.",
+      "exact_quote": "for the ratable benefit and the Secured Parties"
+    },
+    {
+      "location": "Page 65, Article I (Definitions)",
+      "error": "There is a pagination error. The page number is '29', but it should sequentially be '30' after the preceding page (Page 63) which was '28'.",
+      "suggestion": "Correct the page number to '30'.",
+      "exact_quote": "29"
+    },
+    {
+      "location": "Page 65, Article I (Definitions)",
+      "error": "The term 'Base Rate SOFR Determination Day' is used, but the defined term is 'Base Rate Term SOFR Determination Day'. This is an inconsistency or typo.",
+      "suggestion": "Replace 'Base Rate SOFR Determination Day' with 'Base Rate Term SOFR Determination Day'.",
+      "exact_quote": "Base Rate SOFR Determination Day"
+    },
+    {
+      "location": "Page 66, Article I (Definitions)",
+      "error": "There is a pagination error. The page number is '29', but it should sequentially be '31' after the preceding page (Page 65) which was '29'.",
+      "suggestion": "Correct the page number to '31'.",
+      "exact_quote": "29"
+    },
+    {
+      "location": "Page 67, Article I (Definitions)",
+      "error": "Section 4.2(a) is referenced in the definition of 'U.S. Government Securities Business Day', but Article IV is explicitly 'RESERVED' in this document and does not contain a Section 4.2(a). This is likely an incorrect cross-reference.",
+      "suggestion": "Correct the cross-reference to the appropriate section, e.g., Section 6.2(a).",
+      "exact_quote": "Sections 2.3(a), 2.4(c), 4.2(a) and 5.2"
+    },
+    {
+      "location": "Page 75, Section 2.3(a)",
+      "error": "The text uses '(1) U.S. Government Securities Business Day' where a numerical word 'one' is expected, consistent with other numerical spellings in parentheses (e.g., 'three (3)').",
+      "suggestion": "Change '(1)' to 'one'.",
+      "exact_quote": "no later than (1) U.S. Government Securities Business Day"
+    },
+    {
+      "location": "Page 77, Section 2.4(a) and (b)",
+      "error": "Paragraph (b) 'Mandatory Prepayments' is incorrectly formatted as a continuation of the sentence from paragraph (a) 'Repayment on Termination Date' instead of as a new, distinct sub-section.",
+      "suggestion": "Start ' (b) Mandatory Prepayments.' on a new line and ensure it is properly formatted as a separate sub-section.",
+      "exact_quote": "accrued but unpaid interest thereon (b) Mandatory Prepayments."
+    },
+    {
+      "location": "Page 77, Section 2.4(d)",
+      "error": "The section is marked 'Reserved', indicating a placeholder or an incomplete section.",
+      "suggestion": "Either provide content for this section or explicitly state that it is intentionally left blank if it is not a drafting oversight.",
+      "exact_quote": "(d) Reserved."
+    },
+    {
+      "location": "Page 92, Section 5.9",
+      "error": "Section 4.4(a) is referenced in the indemnity clause, but Article IV is explicitly 'RESERVED' in this document and does not contain a Section 4.4(a). This is likely an incorrect cross-reference.",
+      "suggestion": "Correct the cross-reference to the appropriate section, e.g., Section 2.4(c).",
+      "exact_quote": "Section 4.4(a)"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-30 01:28:49</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>d6568581-5567-430e-a7af-ad98d7fd75de.pdf</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+ EX-4.1 3 d45101 1dex41.htm EX-4.1 
+ Exhibit 4.1 
+ CAPIT AL ONE PRIME AUT O RECEIV ABLES TRUST 2023-1 
+ Class A-1 4.900% Auto Loan Asset Backed Notes 
+ Class A-2 5.20% Auto Loan Asset Backed Notes 
+ Class A-3 4.87% Auto Loan Asset Backed Notes 
+ Class A-4 4.76% Auto Loan Asset Backed Notes 
+ Class B 5.07% Auto Loan Asset Backed Notes 
+ Class C 5.36% Auto Loan Asset Backed Notes 
+ Class D 6.34% Auto Loan Asset Backed Notes 
+ INDENTURE 
+ Dated as of February 23, 2023 
+ WILMINGT ON TRUST , NATIONAL ASSOCIA TION, 
+ as the Indenture T rustee 
+--- [START OF PAGE 2] ---
+ CROSS REFERENCE T ABLE  1 
+ TIA  Section  Indenture  Section 
+ 310  (a) (1)  6.11 
+ (a) (2)  6.11 
+ (a) (3)  6.10; 6.1 1 
+ (a) (4)  N.A.  2 
+ (a) (5)  6.11 
+ (b)  6.8; 6.1 1 
+ (c)  N.A. 
+ 311  (a)  6.12 
+ (b)  6.12 
+ (c)  N.A. 
+ 312  (a)  7.1 
+ (b)  7.2 
+ (c)  7.2 
+ 313  (a)  7.3 
+ (b) (1)  7.3 
+ (b) (2)  7.3 
+ (c)  7.3 
+ (d)  7.3 
+ 314  (a)  3.9 
+ (b)  11.1, 3.6 
+ (c) (1)  11.1 
+ (c) (2)  11.1 
+ (c) (3)  11.1 
+ (d)  11.1 
+ (e)  11.1 
+ (f)  N.A. 
+ 315  (a)  6.1(b) 
+ (b)  6.5 
+ (c)  6.1(a) 
+ (d)  6.1(c) 
+ (e)  5.13 
+ 316  (a) (1) (A)  5.11 
+ (a) (1) (B)  5.12 
+ (a) (2)  N.A. 
+ (b)  5.7 
+ (c)  5.6(b) 
+ 317  (a) (1)  5.3(b) 
+ (a) (2)  5.3(d) 
+ (b)  3.3 
+ 318  (a)  11.7 
+ 1  Note: This Cross Reference T able shall not, for  any purpose, be deemed to be part of this Indenture. 
+ 2  N.A. means Not Applicable. 
+ COPAR 2023-1 Indentur e 
+--- [START OF PAGE 3] ---
+ Page 
+ ARTICLE I  DEFINITIONS AND INCORPORA TION BY REFERENCE  2 
+ Section 1.1  Definitions  2 
+ Section 1.2  Incorporation by Reference of T rust Indenture Act  2 
+ Section 1.3  Other Interpretive Provisions  2 
+ ARTICLE II  THE NOTES  3 
+ Section 2.1  Form  3 
+ Section 2.2  Execution, Authentication and Delivery  3 
+ Section 2.3  Temporary Notes  4 
+ Section 2.4  Registration of T ransfer and Exchange  4 
+ Section 2.5  Mutilated, Destroyed, Lost or Stolen Notes  6 
+ Section 2.6  Persons Deemed Owners  6 
+ Section 2.7  Payment of Principal and Interest; Defaulted Interest  7 
+ Section 2.8  Cancellation  7 
+ Section 2.9  Release of Collateral  8 
+ Section 2.10  Book-Entry Notes  8 
+ Section 2.1 1  Notices to Clearing Agency  9 
+ Section 2.12  Definitive Notes  9 
+ Section 2.13  Authenticating Agents  10 
+ Section 2.14  Paying Agent  10 
+ Section 2.15  Tax and Accounting T reatment  11 
+ Section 2.16  Certain T ransfer Restrictions on all Classes of the Notes  11 
+ Section 2.17  Certain T ransfer Restrictions  12 
+ Section 2.18  Transfer Restrictions on Certain Notes Upon a Sale of a Certificate  12 
+ Section 2.19  Certain T ransfer Restrictions on the 144A Notes  13 
+ ARTICLE III  COVENANTS  17 
+ Section 3.1  Payment of Principal and Interest  17 
+ Section 3.2  Maintenance of Of fice or Agency  17 
+ Section 3.3  Money for Payments to Be Held in T rust  17 
+ Section 3.4  Existence  19 
+ Section 3.5  Protection of Collateral  19 
+--- [START OF PAGE 4] ---
+--- [START OF PAGE 5] ---
+ Page 
+ Section 3.6  Opinions as to Collateral  20 
+ Section 3.7  Performance of Obligations; Servicing of Receivables  20 
+ Section 3.8  Negative Covenants  21 
+ Section 3.9  Annual Compliance Statement  22 
+ Section 3.10  Restrictions on Certain Other Activities  23 
+ Section 3.1 1  Restricted Payments  23 
+ Section 3.12  Notice of Events of Default  23 
+ Section 3.13  Further Instruments and Acts  23 
+ Section 3.14  Compliance with Laws  23 
+ Section 3.15  Removal of Administrator  23 
+ Section 3.16  Perfection Representations, W arranties and Covenants  24 
+ Section 3.17  Investment Company Act Representation  24 
+ ARTICLE IV  SATISF ACTION AND DISCHARGE  24 
+ Section 4.1  Satisfaction and Dischar ge of Indenture  24 
+ Section 4.2  Application of T rust Money  25 
+ Section 4.3  Repayment of Monies Held by Paying Agent  25 
+ ARTICLE V  REMEDIES  25 
+ Section 5.1  Events of Default  25 
+ Section 5.2  Acceleration of Maturity; W aiver of Event of Default  26 
+ Section 5.3  Collection of Indebtedness and Suits for Enforcement by the Indenture T rustee  27 
+ Section 5.4  Remedies; Priorities  29 
+ Section 5.5  Optional Preservation of the Collateral  32 
+ Section 5.6  Limitation of Suits  32 
+ Section 5.7  Rights of Noteholders to Receive Principal and Interest  33 
+ Section 5.8  Restoration of Rights and Remedies  33 
+ Section 5.9  Rights and Remedies Cumulative  33 
+ Section 5.10  Delay or Omission Not a W aiver  33 
+ Section 5.1 1  Control by Noteholders  34 
+ Section 5.12  Waiver of Past Defaults  34 
+ Section 5.13  Undertaking for Costs  35 
+--- [START OF PAGE 6] ---
+--- [START OF PAGE 7] ---
+ Page 
+ Section 5.14  Waiver of Stay or Extension Laws  35 
+ Section 5.15  Action on Notes  35 
+ Section 5.16  Performance and Enforcement of Certain Obligations  35 
+ Section 5.17  Sale of Collateral  36 
+ ARTICLE VI  THE INDENTURE TRUSTEE  37 
+ Section 6.1  Duties of the Indenture T rustee  37 
+ Section 6.2  Rights of the Indenture T rustee  38 
+ Section 6.3  Individual Rights of the Indenture T rustee  40 
+ Section 6.4  The Indenture T rustee’ s Disclaimer  40 
+ Section 6.5  Notice of Defaults  40 
+ Section 6.6  Reports by the Paying Agent  40 
+ Section 6.7  Compensation and Indemnity  40 
+ Section 6.8  Removal, Resignation and Replacement of the Indenture T rustee  41 
+ Section 6.9  Successor Indenture T rustee by Mer ger  42 
+ Section 6.10  Appointment of Co-Indenture T rustee or Separate Indenture T rustee  43 
+ Section 6.1 1  Eligibility; Disqualification  44 
+ Section 6.12  Preferential Collection of Claims Against the Issuer  44 
+ Section 6.13  Representations and W arranties  44 
+ ARTICLE VII  NOTEHOLDERS’ LISTS AND REPOR TS  45 
+ Section 7.1  The Issuer to Furnish the Indenture T rustee Names and Addresses of Noteholders  45 
+ Section 7.2  Preservation of Information; Communications to Noteholders  45 
+ Section 7.3  Reports by the Indenture T rustee  45 
+ Section 7.4  Statements to Certificateholders and Noteholders  45 
+ Section 7.5  Noteholder Demand for Repurchase, Dispute Resolution  47 
+ Section 7.6  Investor Action to Initiate an Asset Review  48 
+ ARTICLE VIII  ACCOUNTS, DISBURSEMENTS AND RELEASES  49 
+ Section 8.1  Collection of Money  49 
+ Section 8.2  Trust Accounts  49 
+--- [START OF PAGE 8] ---
+ Page 
+ Section 8.3  General Provisions Regarding Accounts  51 
+ Section 8.4  Additional W ithdrawals and Deposits  54 
+ Section 8.5  Distributions  54 
+ Section 8.6  Release of Collateral  56 
+ Section 8.7  Opinion of Counsel  56 
+ ARTICLE IX  SUPPLEMENT AL INDENTURES  57 
+ Section 9.1  Supplemental Indentures W ithout Consent of Noteholders  57 
+ Section 9.2  Supplemental Indentures with Consent of Noteholders  58 
+ Section 9.3  Execution of Supplemental Indentures  59 
+ Section 9.4  Effect of Supplemental Indenture  60 
+ Section 9.5  Conformity with T rust Indenture Act  60 
+ Section 9.6  Reference in Notes to Supplemental Indentures  60 
+ ARTICLE X  REDEMPTION OF NOTES  60 
+ Section 10.1  Redemption  60 
+ Section 10.2  Form of Redemption Notice  61 
+ Section 10.3  Notes Payable on Redemption Date  61 
+ ARTICLE XI  MISCELLANEOUS  62 
+ Section 1 1.1  Compliance Certificates and Opinions, etc.  62 
+ Section 1 1.2  Form of Documents Delivered to the Indenture T rustee  63 
+ Section 1 1.3  Acts of Noteholders  64 
+ Section 1 1.4  Notices  65 
+ Section 1 1.5  Notices to Noteholders; W aiver  65 
+ Section 1 1.6  Alternate Payment and Notice Provisions  65 
+ Section 1 1.7  Conflict with T rust Indenture Act  65 
+ Section 1 1.8  Information Requests  66 
+ Section 1 1.9  Effect of Headings and T able of Contents  66 
+ Section 1 1.10  Successors and Assigns  66 
+ Section 1 1.11  Separability  66 
+ Section 1 1.12  Benefits of Indenture  66 
+ Section 1 1.13  Legal Holidays  66 
+--- [START OF PAGE 9] ---
+--- [START OF PAGE 10] ---
+ Page 
+ Section 1 1.14  GOVERNING LA W  66 
+ Section 1 1.15  Counterparts  66 
+ Section 1 1.16  Recording of Indenture  67 
+ Section 1 1.17  Trust Obligation  67 
+ Section 1 1.18  No Petition  67 
+ Section 1 1.19  Submission to Jurisdiction; W aiver of Jury T rial  68 
+ Section 1 1.20  Subordination of Claims  68 
+ Section 1 1.21  U.S.A Patriot Act  69 
+ Section 1 1.22  Beneficial Ownership  69 
+ Section 1 1.23  Limitation of Liability  69 
+ ARTICLE XII  COMPLIANCE WITH THE FDIC RULE  70 
+ Section 12.1  Purpose  70 
+ Section 12.2  Requirements of the FDIC Rule  71 
+ Section 12.3  Performance  72 
+ Section 12.4  Actions Upon Repudiation  73 
+ Section 12.5  Notice  75 
+ Section 12.6  Reservation of Rights  75 
+ Schedule I  Perfection Representations, W arranties and Covenants 
+ Exhibit A  Form of Notes 
+--- [START OF PAGE 11] ---
+ This INDENTURE, dated as of February 28, 2023 (as amended, supplemented, or otherwise modified and in ef fect from time to time, this 
+ “  Indenture  ”), is between CAPIT AL ONE PRIME AUT O RECEIV ABLES  TRUST 2023-1, a Delaware statutory trust (the “  Issuer  ”),  and W ilmington 
+ Trust, National Association, a national banking association, solely as trustee and not in its individual capacity (the “  Indenture T rustee  ”). 
+ Each party agrees as follows for the benefit of the other party and the equal and ratable benefit of the Holders of the Issuer ’s Class A-1 
+ 4.900% Auto Loan Asset Backed Notes (the “  Class A-1  Notes  ”), Class A-2 5.20% Auto Loan Asset Backed Notes  (the “  Class A-2 Notes  ”), Class 
+ A-3 4.87% Auto Loan Asset Backed Notes (the “  Class  A-3 Notes  ”), Class A-4 4.76% Auto Loan Asset Backed  Notes (the “  Class A-4 Notes  ”, and 
+ together with the Class A-1 Notes, the Class A-2 Notes and the Class A-3 Notes, the “  Class A Notes  ”), Class  B 5.07% Auto Loan Asset Backed 
+ Notes (the “  Class B Notes  ”), Class C 5.36% Auto Loan  Asset Backed Notes (the “  Class C Notes  ”) and Class  D 6.34% Auto Loan Asset Backed 
+ Notes (the “  Class D Notes  ”, and together with the  Class A-1 Notes, the Class A-2 Notes, the Class A-3 Notes, the Class A-4 Notes, the Class B Notes 
+ and the Class C Notes, the “  Notes  ”). 
+ GRANTING CLAUSE 
+ The Issuer , to secure the payment of principal of and interest on, and any other amounts owing in respect of, the Notes equally and ratably 
+ without prejudice, priority or distinction except as set forth herein, and to secure compliance with the provisions of this Indenture, hereby Grants in trust 
+ to the Indenture T rustee on the Closing Date, as trustee for the benefit of the Noteholders, all of the Issuer ’s right, title and interest, whether now owned 
+ or hereafter acquired, in and to (i) the T rust Estate and (ii) all present and future claims, demands, causes and choses in action in respect of any or all of 
+ the T rust Estate and all payments on or under and all proceeds of every kind and nature whatsoever in respect of any or all of the T rust Estate, including 
+ all proceeds of the conversion, voluntary or involuntary , into cash or other liquid property , all cash proceeds, accounts, accounts receivable, notes, drafts, 
+ acceptances, chattel paper , checks, deposit accounts, insurance proceeds, condemnation awards, rights to payment of any and every kind and other forms 
+ of obligations and receivables, instruments, securities, financial assets and other property which at any time constitute all or part of or are included in the 
+ proceeds of any of the T rust Estate (collectively , the “  Collateral  ”). 
+ The Indenture T rustee, on behalf of the Noteholders, acknowledges the foregoing Grant, accepts the trusts under this Indenture and 
+ agrees to perform its duties required in this Indenture in accordance with the provisions of this Indenture. 
+ The foregoing Grant is made in trust to secure (i) the payment of principal of and interest on, and any other amounts owing in respect of, 
+ the Notes, equally and ratably without prejudice, priority or distinction except as set forth herein and (ii) compliance with the provisions of this 
+ Indenture, all as provided in this Indenture. 
+ Without limiting the foregoing Grant, any Receivable repurchased or purchased by (a) the Servicer pursuant to  Section 3.6  of the Servicing 
+ Agreement or (b) by the Bank pursuant to  Section 3.4  of the Purchase Agreement shall be deemed to be automatically released from the lien of this 
+ Indenture without any action being taken by the Indenture T rustee upon payment by the applicable purchaser of the related Repurchase Price for such 
+ Repurchased Receivable. 
+ COPAR 2023-1 Indentur e 
+--- [START OF PAGE 12] ---
+ ARTICLE I 
+ DEFINITIONS AND INCORPORA TION BY REFERENCE 
+ SECTION 1.1  Definitions  . Capitalized terms are used  in this Indenture as defined in  A  p  p  endix A  to the  Sale Agreement, dated as of the 
+ date hereof (as amended, supplemented, or otherwise modified and in ef fect from time to time, the “  Sale  Agreement  ”), between the Issuer and Capital 
+ One Auto Receivables, LLC, which also contains rules as to usage that are applicable herein. 
+ SECTION 1.2  Incorporation by Reference of T rust Indenture  Act  . Whenever this Indenture refers to a provision  of the TIA, the provision 
+ is incorporated by reference in and made a part of this Indenture. The following TIA terms used in this Indenture have the following meanings: 
+ “  Commission  ” means the Securities and Exchange Commission. 
+ “  indenture securities  ” means the Notes. 
+ “  indenture securi  ty  holder  ” means a Noteholder . 
+ “  indenture to be qualified  ” means this Indenture. 
+ “  indenture trustee  ” or “  institutional trustee  ” means  the Indenture T rustee. 
+ “  obl  ig  or  ” on the indenture securities means the Issuer  and any other obligor on the indenture securities. 
+ All other TIA terms used in this Indenture that are defined by the TIA, defined by TIA reference to another statute or defined by 
+ Commission rule have the meaning assigned to them by such definitions. 
+ SECTION 1.3  Other Interpretive Provisions  . All terms  defined in this Indenture shall have the defined meanings when used in any 
+ certificate or other document delivered pursuant hereto unless otherwise defined therein. For purposes of this Indenture and all such certificates and 
+ other documents, unless the context otherwise requires: (a) accounting terms not otherwise defined in this Indenture, and accounting terms partly 
+ defined in this Indenture to the extent not defined, shall have the respective meanings given to them under GAAP (  provided  , that, to the extent that the 
+ definitions in this Indenture and GAAP conflict, the definitions in this Indenture shall control); (b) terms defined in Article 9 of the UCC as in ef fect in 
+ the relevant jurisdiction and not otherwise defined in this Indenture are used as defined in that Article; (c) the words “hereof,” “herein” and “hereunder” 
+ and words of similar import refer to this Indenture as a whole and not to any particular provision of this Indenture; (d) references to any Article, 
+ Section, Schedule, Appendix or Exhibit are references to Articles, Sections, Schedules, Appendices and Exhibits in or to this Indenture and references 
+ to any paragraph, subsection, clause or other subdivision within any Section or definition refer to such paragraph, subsection, clause or other 
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.11",
+      "error": "The capitalized term 'Clearing Agency' is used but not defined within this document. While Section 1.1 points to an external document for definitions, as a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Clearing Agency' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 2.11 Notices to Clearing Agency"
+    },
+    {
+      "location": "Page 3, Section 2.12",
+      "error": "The capitalized term 'Definitive Notes' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Definitive Notes' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 2.12 Definitive Notes"
+    },
+    {
+      "location": "Page 3, Section 2.13",
+      "error": "The capitalized term 'Authenticating Agents' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Authenticating Agents' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 2.13 Authenticating Agents"
+    },
+    {
+      "location": "Page 3, Section 2.14",
+      "error": "The capitalized term 'Paying Agent' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Paying Agent' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 2.14 Paying Agent"
+    },
+    {
+      "location": "Page 3, Section 2.18",
+      "error": "The capitalized term 'Certificate' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Certificate' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 2.18 Transfer Restrictions on Certain Notes Upon a Sale of a Certificate"
+    },
+    {
+      "location": "Page 3, Section 2.19",
+      "error": "The capitalized term '144A Notes' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for '144A Notes' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 2.19 Certain Transfer Restrictions on the 144A Notes"
+    },
+    {
+      "location": "Page 5, Section 3.7",
+      "error": "The capitalized term 'Receivables' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Receivables' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 3.7 Performance of Obligations; Servicing of Receivables"
+    },
+    {
+      "location": "Page 5, Section 3.11",
+      "error": "The capitalized term 'Restricted Payments' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Restricted Payments' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 3.11 Restricted Payments"
+    },
+    {
+      "location": "Page 5, Section 3.12",
+      "error": "The capitalized term 'Events of Default' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Events of Default' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 3.12 Notice of Events of Default"
+    },
+    {
+      "location": "Page 5, Section 3.15",
+      "error": "The capitalized term 'Administrator' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Administrator' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 3.15 Removal of Administrator"
+    },
+    {
+      "location": "Page 5, Section 4.2",
+      "error": "The capitalized term 'Trust Money' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Trust Money' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 4.2 Application of Trust Money"
+    },
+    {
+      "location": "Page 5, Section 5.3",
+      "error": "The capitalized term 'Indebtedness' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Indebtedness' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 5.3 Collection of Indebtedness and Suits for Enforcement by the Indenture Trustee"
+    },
+    {
+      "location": "Page 5, Section 5.7",
+      "error": "The capitalized term 'Noteholders' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Noteholders' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 5.7 Rights of Noteholders to Receive Principal and Interest"
+    },
+    {
+      "location": "Page 5, Section 5.12",
+      "error": "The capitalized term 'Past Defaults' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Past Defaults' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 5.12 Waiver of Past Defaults"
+    },
+    {
+      "location": "Page 7, Section 6.9",
+      "error": "The capitalized term 'Merger' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Merger' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 6.9 Successor Indenture Trustee by Mer ger"
+    },
+    {
+      "location": "Page 7, Section 6.10",
+      "error": "The capitalized term 'Co-Indenture Trustee' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Co-Indenture Trustee' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 6.10 Appointment of Co-Indenture T rustee or Separate Indenture T rustee"
+    },
+    {
+      "location": "Page 7, Section 6.10",
+      "error": "The capitalized term 'Separate Indenture Trustee' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Separate Indenture Trustee' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 6.10 Appointment of Co-Indenture T rustee or Separate Indenture T rustee"
+    },
+    {
+      "location": "Page 7, Section 7.4",
+      "error": "The capitalized term 'Certificateholders' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Certificateholders' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 7.4 Statements to Certificateholders and Noteholders"
+    },
+    {
+      "location": "Page 7, Section 7.5",
+      "error": "The capitalized term 'Repurchase' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Repurchase' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 7.5 Noteholder Demand for Repurchase, Dispute Resolution"
+    },
+    {
+      "location": "Page 7, Section 7.6",
+      "error": "The capitalized term 'Investor' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Investor' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 7.6 Investor Action to Initiate an Asset Review"
+    },
+    {
+      "location": "Page 7, Section 7.6",
+      "error": "The capitalized term 'Asset Review' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Asset Review' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 7.6 Investor Action to Initiate an Asset Review"
+    },
+    {
+      "location": "Page 7, Section 8.2",
+      "error": "The capitalized term 'Trust Accounts' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Trust Accounts' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 8.2 Trust Accounts"
+    },
+    {
+      "location": "Page 8, Section 8.5",
+      "error": "The capitalized term 'Distributions' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Distributions' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 8.5 Distributions"
+    },
+    {
+      "location": "Page 8, Section 10.1",
+      "error": "The capitalized term 'Redemption' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Redemption' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 10.1 Redemption"
+    },
+    {
+      "location": "Page 8, Section 10.2",
+      "error": "The capitalized term 'Redemption Notice' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Redemption Notice' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 10.2 Form of Redemption Notice"
+    },
+    {
+      "location": "Page 8, Section 10.3",
+      "error": "The capitalized term 'Redemption Date' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Redemption Date' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 10.3 Notes Payable on Redemption Date"
+    },
+    {
+      "location": "Page 8, Section 11.13",
+      "error": "The capitalized term 'Legal Holidays' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Legal Holidays' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 11.13 Legal Holidays"
+    },
+    {
+      "location": "Page 10, Section 11.14",
+      "error": "The capitalized term 'GOVERNING LAW' is used but not defined within this document. Additionally, section titles in the Table of Contents should typically be Title Case for consistency (e.g., 'Governing Law').",
+      "suggestion": "Either provide a definition for 'Governing Law' in this document or explicitly state its definition by reference within the relevant section. Also, revise the capitalization of the section title in the Table of Contents to 'Governing Law'.",
+      "exact_quote": "Section 11.14 GOVERNING LA W"
+    },
+    {
+      "location": "Page 10, Section 11.19",
+      "error": "The capitalized term 'Jury Trial' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Jury Trial' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 11.19 Submission to Jurisdiction; W aiver of Jury T rial"
+    },
+    {
+      "location": "Page 10, Section 11.21",
+      "error": "The capitalized term 'U.S.A Patriot Act' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'U.S.A Patriot Act' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 11.21 U.S.A Patriot Act"
+    },
+    {
+      "location": "Page 10, Section 12.2",
+      "error": "The capitalized term 'FDIC Rule' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'FDIC Rule' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 12.2 Requirements of the FDIC Rule"
+    },
+    {
+      "location": "Page 10, Section 12.4",
+      "error": "The capitalized term 'Repudiation' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Repudiation' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 12.4 Actions Upon Repudiation"
+    },
+    {
+      "location": "Page 11, Introductory Paragraph",
+      "error": "The capitalized term 'Holders' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition. It should ideally be consistently 'Noteholders' or explicitly defined.",
+      "suggestion": "Either define 'Holders' or consistently use 'Noteholders' throughout the document. If used interchangeably, a definition confirming this should be provided.",
+      "exact_quote": "for the benefit of the other party and the equal and ratable benefit of the Holders of the Issuer’s Class A-1"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The word 'Grants' is incorrectly capitalized as a verb. It should be lowercase.",
+      "suggestion": "Change 'Grants' to 'grants'.",
+      "exact_quote": "hereby Grants in trust"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Closing Date' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Closing Date' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "to the Indenture T rustee on the Closing Date"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Trust Estate' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Trust Estate' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "in and to (i) the T rust Estate"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Servicer' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Servicer' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "by (a) the Servicer pursuant to Section 3.6 of the Servicing Agreement"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Servicing Agreement' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Servicing Agreement' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 3.6 of the Servicing Agreement"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Bank' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Bank' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "or (b) by the Bank pursuant to Section 3.4 of the Purchase Agreement"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Purchase Agreement' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Purchase Agreement' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "Section 3.4 of the Purchase Agreement"
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Repurchase Price' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Repurchase Price' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "of the related Repurchase Price for such Repurchased Receivable."
+    },
+    {
+      "location": "Page 11, Granting Clause",
+      "error": "The capitalized term 'Repurchased Receivable' is used but not defined within this document. As a standalone document fragment, a reader cannot access the definition.",
+      "suggestion": "Either provide a definition for 'Repurchased Receivable' in this document or explicitly state its definition by reference within the relevant section.",
+      "exact_quote": "of the related Repurchase Price for such Repurchased Receivable."
+    },
+    {
+      "location": "Page 12, Section 1.3",
+      "error": "The capitalized term 'UCC' is used but not defined within this document. While Section 1.3 points to Article 9 of the UCC for definitions, as a standalone document fragment, a reader cannot access the definition or confirm what 'UCC' refers to without external knowledge.",
+      "suggestion": "Either provide a definition for 'UCC' (e.g., Uniform Commercial Code) in this document or explicitly define its meaning by reference within the relevant section.",
+      "exact_quote": "Article 9 of the UCC as in ef fect in the relevant jurisdiction"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added locator swarm anime and locator will now work in parallel. Although sometimes it misses when highlighting exact text
</commit_message>
<xml_diff>
--- a/backend/audit_logs.xlsx
+++ b/backend/audit_logs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3792,6 +3792,1064 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-30 02:51:08</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>c7c4e665-856c-4e55-a8c5-a4a3cc1708d6.pdf</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "ARTICLE I: DEFINITIONS, \"Applicable Margin\"",
+      "error": "The Consolidated Total Leverage Ratio ranges in the \"Applicable Margin\" table contain a gap. A ratio greater than or equal to 2.50 to 1.00 but less than 2.60 to 1.00 is not covered by any pricing level, specifically falling between Pricing Level II and Pricing Level III.",
+      "suggestion": "Adjust the ranges in the 'Consolidated Total Leverage Ratio' column to ensure continuous coverage without gaps or overlaps. For example, change Level III to 'Greater than or equal to 1.75 to 1.00 but less than 2.60 to 1.00'.",
+      "exact_quote": "Consolidated Total Leverage Ratio\nSOFR Margin\nI\nGreater than or equal to 3.25 to 1.00\n2.75%\nII\nGreater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00\n2.50%\nIII\nGreater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00\n2.25%\nIV\nGreater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00\n2.00%\nV\nLess than 1.50 to 1.00\n1.75%"
+    },
+    {
+      "location": "SECTION 2.5 Permanent Reduction of the Revolving Credit Commitment",
+      "error": "The capitalized term \"Cash Collateralization\" is used in this section but is not defined in the document.",
+      "suggestion": "Define \"Cash Collateralization\" in Article I (DEFINITIONS) or rephrase the sentence to avoid using an undefined capitalized term.",
+      "exact_quote": "Cash Collateralization"
+    },
+    {
+      "location": "SECTION 5.13 Incremental Loans",
+      "error": "A placeholder \"[__]\" remains in the text, indicating an incomplete detail.",
+      "suggestion": "Replace the placeholder with the intended location of the Administrative Agent's office.",
+      "exact_quote": "[__]"
+    },
+    {
+      "location": "SECTION 5.13 Incremental Loans",
+      "error": "The capitalized term \"Incremental Revolving Credit Increase\" is used but is not formally defined in the document. While 'increases in the Revolving Credit Commitments' is mentioned, 'Incremental Revolving Credit Increase' is used as a distinct capitalized term without a definition.",
+      "suggestion": "Define \"Incremental Revolving Credit Increase\" in Article I (DEFINITIONS), or ensure consistent use of 'increases in the Revolving Credit Commitments' throughout the section.",
+      "exact_quote": "Incremental Revolving Credit Increase"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-30 13:27:52</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ecf6fb9e-494e-4722-89a1-e841c0ebfcc5.pdf</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, ARTICLE I: DEFINITIONS, Applicable Margin",
+      "error": "The pricing table for 'Applicable Margin' contains a logical gap in the 'Consolidated Total Leverage Ratio' ranges. Ratios greater than or equal to 2.50 to 1.00 but less than 2.60 to 1.00 are not covered by any pricing level.",
+      "suggestion": "Adjust the ranges for Level II or Level III to ensure continuous coverage of all possible ratios. For example, Level III could be 'Greater than or equal to 1.75 to 1.00 but less than 2.60 to 1.00' or Level II could be 'Greater than or equal to 2.50 to 1.00 but less than 3.25 to 1.00'.",
+      "exact_quote": "II Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00\nIII Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00"
+    },
+    {
+      "location": "Page 1, SECTION 2.5",
+      "error": "The capitalized term \"Cash Collateralization\" is used in Section 2.5 but is not defined in the provided document fragment, despite the note indicating that \"Cash Collateralize\" is defined.",
+      "suggestion": "Add a definition for \"Cash Collateralization\" in ARTICLE I: DEFINITIONS, or revise the text to use an already defined term like \"Cash Collateral\" (if applicable).",
+      "exact_quote": "Cash Collateralization satisfactory to the Administrative Agent."
+    },
+    {
+      "location": "Page 1, SECTION 5.13",
+      "error": "The capitalized term \"First Amendment Effective Date\" is used in Section 5.13 but is not defined in the provided document fragment. This is a deal-specific term that requires a definition.",
+      "suggestion": "Add a definition for \"First Amendment Effective Date\" in ARTICLE I: DEFINITIONS.",
+      "exact_quote": "At any time after the First Amendment Effective Date, the Borrower may by written notice to the"
+    },
+    {
+      "location": "Page 2, SECTION 5.13",
+      "error": "The capitalized term \"Incremental Revolving Credit Increase\" is used in Section 5.13 but is not defined in the provided document fragment.",
+      "suggestion": "Add a definition for \"Incremental Revolving Credit Increase\" in ARTICLE I: DEFINITIONS.",
+      "exact_quote": "The terms of such Incremental Revolving Credit Increase shall be subject to the documentation"
+    },
+    {
+      "location": "Page 2, SECTION 5.13",
+      "error": "A placeholder \"[__]\" is present, indicating that the location of the Administrative Agent's office has not been specified.",
+      "suggestion": "Replace \"[__]\" with the specific location of the Administrative Agent's office.",
+      "exact_quote": "at its office in [__] (or such other location as"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-30 13:29:02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>b38b6cf0-024f-4081-9bd4-40c725d901c8.pdf</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>{
+  "errors": []
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-30 13:59:23</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>c92d18a1-8b01-49ac-8b4b-1f7b9436b852.pdf</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, ARTICLE I: DEFINITIONS",
+      "error": "The definition of 'Cash Collateral' relies on 'the foregoing' which is not provided or defined within this document fragment, making the definition incomplete or circular in isolation.",
+      "suggestion": "Provide a complete, standalone definition for 'Cash Collateral' or ensure 'the foregoing' is clearly defined prior to this term.",
+      "exact_quote": "\"Cash Collateral\" shall have a meaning correlative to the foregoing and shall include the proceeds of such cash collateral..."
+    },
+    {
+      "location": "Page 1, SECTION 2.5",
+      "error": "The capitalized term 'Cash Collateralization' is used but not defined.",
+      "suggestion": "Add a definition for 'Cash Collateralization' in ARTICLE I: DEFINITIONS.",
+      "exact_quote": "furnishing of Cash Collateralization satisfactory to the Administrative Agent."
+    },
+    {
+      "location": "Page 1, SECTION 5.13",
+      "error": "The capitalized term 'First Amendment Effective Date' is used but not defined.",
+      "suggestion": "Add a definition for 'First Amendment Effective Date' in ARTICLE I: DEFINITIONS.",
+      "exact_quote": "At any time after the First Amendment Effective Date, the Borrower may by written notice to the Administrative Agent elect to request the establishment of one or more increases in the Revolving"
+    },
+    {
+      "location": "Page 2, SECTION 5.13",
+      "error": "A placeholder '[__]' has been left in the text.",
+      "suggestion": "Fill in the missing information for the Administrative Agent's office location.",
+      "exact_quote": "Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as the Administrative Agent may designate)."
+    },
+    {
+      "location": "Page 2, SECTION 5.13",
+      "error": "The capitalized term 'Incremental Revolving Credit Increase' is used but not defined.",
+      "suggestion": "Add a definition for 'Incremental Revolving Credit Increase' in ARTICLE I: DEFINITIONS.",
+      "exact_quote": "The terms of such Incremental Revolving Credit Increase shall be subject to the documentation requirements set forth in Section 5.19."
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-30 15:41:53</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>bb4d1ef1-f076-4ab0-905f-ec62a47e24b1.pdf</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, Article I: Definitions",
+      "error": "Undefined capitalized term 'Cash Collateralization' is used.",
+      "suggestion": "Define 'Cash Collateralization' in the definitions section or replace with a defined term.",
+      "exact_quote": "furnishing of Cash Collateralization satisfactory to the Administrative Agent."
+    },
+    {
+      "location": "Page 2, Section 5.13",
+      "error": "Placeholder not filled out for the location of Administrative Agent's office.",
+      "suggestion": "Provide the specific location for the Administrative Agent's office.",
+      "exact_quote": "at its office in [__]"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-30 15:43:36</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>fb0d1b61-774a-4b06-9c54-9c7f21f67010.pdf</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+ EX-4.1 3 d45101 1dex41.htm EX-4.1 
+ Exhibit 4.1 
+ CAPIT AL ONE PRIME AUT O RECEIV ABLES TRUST 2023-1 
+ Class A-1 4.900% Auto Loan Asset Backed Notes 
+ Class A-2 5.20% Auto Loan Asset Backed Notes 
+ Class A-3 4.87% Auto Loan Asset Backed Notes 
+ Class A-4 4.76% Auto Loan Asset Backed Notes 
+ Class B 5.07% Auto Loan Asset Backed Notes 
+ Class C 5.36% Auto Loan Asset Backed Notes 
+ Class D 6.34% Auto Loan Asset Backed Notes 
+ INDENTURE 
+ Dated as of February 23, 2023 
+ WILMINGT ON TRUST , NATIONAL ASSOCIA TION, 
+ as the Indenture T rustee 
+--- [START OF PAGE 2] ---
+ CROSS REFERENCE T ABLE  1 
+ TIA  Section  Indenture  Section 
+ 310  (a) (1)  6.11 
+ (a) (2)  6.11 
+ (a) (3)  6.10; 6.1 1 
+ (a) (4)  N.A.  2 
+ (a) (5)  6.11 
+ (b)  6.8; 6.1 1 
+ (c)  N.A. 
+ 311  (a)  6.12 
+ (b)  6.12 
+ (c)  N.A. 
+ 312  (a)  7.1 
+ (b)  7.2 
+ (c)  7.2 
+ 313  (a)  7.3 
+ (b) (1)  7.3 
+ (b) (2)  7.3 
+ (c)  7.3 
+ (d)  7.3 
+ 314  (a)  3.9 
+ (b)  11.1, 3.6 
+ (c) (1)  11.1 
+ (c) (2)  11.1 
+ (c) (3)  11.1 
+ (d)  11.1 
+ (e)  11.1 
+ (f)  N.A. 
+ 315  (a)  6.1(b) 
+ (b)  6.5 
+ (c)  6.1(a) 
+ (d)  6.1(c) 
+ (e)  5.13 
+ 316  (a) (1) (A)  5.11 
+ (a) (1) (B)  5.12 
+ (a) (2)  N.A. 
+ (b)  5.7 
+ (c)  5.6(b) 
+ 317  (a) (1)  5.3(b) 
+ (a) (2)  5.3(d) 
+ (b)  3.3 
+ 318  (a)  11.7 
+ 1  Note: This Cross Reference T able shall not, for  any purpose, be deemed to be part of this Indenture. 
+ 2  N.A. means Not Applicable. 
+ COPAR 2023-1 Indentur e 
+--- [START OF PAGE 3] ---
+ Page 
+ ARTICLE I  DEFINITIONS AND INCORPORA TION BY REFERENCE  2 
+ Section 1.1  Definitions  2 
+ Section 1.2  Incorporation by Reference of T rust Indenture Act  2 
+ Section 1.3  Other Interpretive Provisions  2 
+ ARTICLE II  THE NOTES  3 
+ Section 2.1  Form  3 
+ Section 2.2  Execution, Authentication and Delivery  3 
+ Section 2.3  Temporary Notes  4 
+ Section 2.4  Registration of T ransfer and Exchange  4 
+ Section 2.5  Mutilated, Destroyed, Lost or Stolen Notes  6 
+ Section 2.6  Persons Deemed Owners  6 
+ Section 2.7  Payment of Principal and Interest; Defaulted Interest  7 
+ Section 2.8  Cancellation  7 
+ Section 2.9  Release of Collateral  8 
+ Section 2.10  Book-Entry Notes  8 
+ Section 2.1 1  Notices to Clearing Agency  9 
+ Section 2.12  Definitive Notes  9 
+ Section 2.13  Authenticating Agents  10 
+ Section 2.14  Paying Agent  10 
+ Section 2.15  Tax and Accounting T reatment  11 
+ Section 2.16  Certain T ransfer Restrictions on all Classes of the Notes  11 
+ Section 2.17  Certain T ransfer Restrictions  12 
+ Section 2.18  Transfer Restrictions on Certain Notes Upon a Sale of a Certificate  12 
+ Section 2.19  Certain T ransfer Restrictions on the 144A Notes  13 
+ ARTICLE III  COVENANTS  17 
+ Section 3.1  Payment of Principal and Interest  17 
+ Section 3.2  Maintenance of Of fice or Agency  17 
+ Section 3.3  Money for Payments to Be Held in T rust  17 
+ Section 3.4  Existence  19 
+ Section 3.5  Protection of Collateral  19 
+--- [START OF PAGE 4] ---
+--- [START OF PAGE 5] ---
+ Page 
+ Section 3.6  Opinions as to Collateral  20 
+ Section 3.7  Performance of Obligations; Servicing of Receivables  20 
+ Section 3.8  Negative Covenants  21 
+ Section 3.9  Annual Compliance Statement  22 
+ Section 3.10  Restrictions on Certain Other Activities  23 
+ Section 3.1 1  Restricted Payments  23 
+ Section 3.12  Notice of Events of Default  23 
+ Section 3.13  Further Instruments and Acts  23 
+ Section 3.14  Compliance with Laws  23 
+ Section 3.15  Removal of Administrator  23 
+ Section 3.16  Perfection Representations, W arranties and Covenants  24 
+ Section 3.17  Investment Company Act Representation  24 
+ ARTICLE IV  SATISF ACTION AND DISCHARGE  24 
+ Section 4.1  Satisfaction and Dischar ge of Indenture  24 
+ Section 4.2  Application of T rust Money  25 
+ Section 4.3  Repayment of Monies Held by Paying Agent  25 
+ ARTICLE V  REMEDIES  25 
+ Section 5.1  Events of Default  25 
+ Section 5.2  Acceleration of Maturity; W aiver of Event of Default  26 
+ Section 5.3  Collection of Indebtedness and Suits for Enforcement by the Indenture T rustee  27 
+ Section 5.4  Remedies; Priorities  29 
+ Section 5.5  Optional Preservation of the Collateral  32 
+ Section 5.6  Limitation of Suits  32 
+ Section 5.7  Rights of Noteholders to Receive Principal and Interest  33 
+ Section 5.8  Restoration of Rights and Remedies  33 
+ Section 5.9  Rights and Remedies Cumulative  33 
+ Section 5.10  Delay or Omission Not a W aiver  33 
+ Section 5.1 1  Control by Noteholders  34 
+ Section 5.12  Waiver of Past Defaults  34 
+ Section 5.13  Undertaking for Costs  35 
+--- [START OF PAGE 6] ---
+--- [START OF PAGE 7] ---
+ Page 
+ Section 5.14  Waiver of Stay or Extension Laws  35 
+ Section 5.15  Action on Notes  35 
+ Section 5.16  Performance and Enforcement of Certain Obligations  35 
+ Section 5.17  Sale of Collateral  36 
+ ARTICLE VI  THE INDENTURE TRUSTEE  37 
+ Section 6.1  Duties of the Indenture T rustee  37 
+ Section 6.2  Rights of the Indenture T rustee  38 
+ Section 6.3  Individual Rights of the Indenture T rustee  40 
+ Section 6.4  The Indenture T rustee’ s Disclaimer  40 
+ Section 6.5  Notice of Defaults  40 
+ Section 6.6  Reports by the Paying Agent  40 
+ Section 6.7  Compensation and Indemnity  40 
+ Section 6.8  Removal, Resignation and Replacement of the Indenture T rustee  41 
+ Section 6.9  Successor Indenture T rustee by Mer ger  42 
+ Section 6.10  Appointment of Co-Indenture T rustee or Separate Indenture T rustee  43 
+ Section 6.1 1  Eligibility; Disqualification  44 
+ Section 6.12  Preferential Collection of Claims Against the Issuer  44 
+ Section 6.13  Representations and W arranties  44 
+ ARTICLE VII  NOTEHOLDERS’ LISTS AND REPOR TS  45 
+ Section 7.1  The Issuer to Furnish the Indenture T rustee Names and Addresses of Noteholders  45 
+ Section 7.2  Preservation of Information; Communications to Noteholders  45 
+ Section 7.3  Reports by the Indenture T rustee  45 
+ Section 7.4  Statements to Certificateholders and Noteholders  45 
+ Section 7.5  Noteholder Demand for Repurchase, Dispute Resolution  47 
+ Section 7.6  Investor Action to Initiate an Asset Review  48 
+ ARTICLE VIII  ACCOUNTS, DISBURSEMENTS AND RELEASES  49 
+ Section 8.1  Collection of Money  49 
+ Section 8.2  Trust Accounts  49 
+--- [START OF PAGE 8] ---
+ Page 
+ Section 8.3  General Provisions Regarding Accounts  51 
+ Section 8.4  Additional W ithdrawals and Deposits  54 
+ Section 8.5  Distributions  54 
+ Section 8.6  Release of Collateral  56 
+ Section 8.7  Opinion of Counsel  56 
+ ARTICLE IX  SUPPLEMENT AL INDENTURES  57 
+ Section 9.1  Supplemental Indentures W ithout Consent of Noteholders  57 
+ Section 9.2  Supplemental Indentures with Consent of Noteholders  58 
+ Section 9.3  Execution of Supplemental Indentures  59 
+ Section 9.4  Effect of Supplemental Indenture  60 
+ Section 9.5  Conformity with T rust Indenture Act  60 
+ Section 9.6  Reference in Notes to Supplemental Indentures  60 
+ ARTICLE X  REDEMPTION OF NOTES  60 
+ Section 10.1  Redemption  60 
+ Section 10.2  Form of Redemption Notice  61 
+ Section 10.3  Notes Payable on Redemption Date  61 
+ ARTICLE XI  MISCELLANEOUS  62 
+ Section 1 1.1  Compliance Certificates and Opinions, etc.  62 
+ Section 1 1.2  Form of Documents Delivered to the Indenture T rustee  63 
+ Section 1 1.3  Acts of Noteholders  64 
+ Section 1 1.4  Notices  65 
+ Section 1 1.5  Notices to Noteholders; W aiver  65 
+ Section 1 1.6  Alternate Payment and Notice Provisions  65 
+ Section 1 1.7  Conflict with T rust Indenture Act  65 
+ Section 1 1.8  Information Requests  66 
+ Section 1 1.9  Effect of Headings and T able of Contents  66 
+ Section 1 1.10  Successors and Assigns  66 
+ Section 1 1.11  Separability  66 
+ Section 1 1.12  Benefits of Indenture  66 
+ Section 1 1.13  Legal Holidays  66 
+--- [START OF PAGE 9] ---
+--- [START OF PAGE 10] ---
+ Page 
+ Section 1 1.14  GOVERNING LA W  66 
+ Section 1 1.15  Counterparts  66 
+ Section 1 1.16  Recording of Indenture  67 
+ Section 1 1.17  Trust Obligation  67 
+ Section 1 1.18  No Petition  67 
+ Section 1 1.19  Submission to Jurisdiction; W aiver of Jury T rial  68 
+ Section 1 1.20  Subordination of Claims  68 
+ Section 1 1.21  U.S.A Patriot Act  69 
+ Section 1 1.22  Beneficial Ownership  69 
+ Section 1 1.23  Limitation of Liability  69 
+ ARTICLE XII  COMPLIANCE WITH THE FDIC RULE  70 
+ Section 12.1  Purpose  70 
+ Section 12.2  Requirements of the FDIC Rule  71 
+ Section 12.3  Performance  72 
+ Section 12.4  Actions Upon Repudiation  73 
+ Section 12.5  Notice  75 
+ Section 12.6  Reservation of Rights  75 
+ Schedule I  Perfection Representations, W arranties and Covenants 
+ Exhibit A  Form of Notes 
+--- [START OF PAGE 11] ---
+ This INDENTURE, dated as of February 28, 2023 (as amended, supplemented, or otherwise modified and in ef fect from time to time, this 
+ “  Indenture  ”), is between CAPIT AL ONE PRIME AUT O RECEIV ABLES  TRUST 2023-1, a Delaware statutory trust (the “  Issuer  ”),  and W ilmington 
+ Trust, National Association, a national banking association, solely as trustee and not in its individual capacity (the “  Indenture T rustee  ”). 
+ Each party agrees as follows for the benefit of the other party and the equal and ratable benefit of the Holders of the Issuer ’s Class A-1 
+ 4.900% Auto Loan Asset Backed Notes (the “  Class A-1  Notes  ”), Class A-2 5.20% Auto Loan Asset Backed Notes  (the “  Class A-2 Notes  ”), Class 
+ A-3 4.87% Auto Loan Asset Backed Notes (the “  Class  A-3 Notes  ”), Class A-4 4.76% Auto Loan Asset Backed  Notes (the “  Class A-4 Notes  ”, and 
+ together with the Class A-1 Notes, the Class A-2 Notes and the Class A-3 Notes, the “  Class A Notes  ”), Class  B 5.07% Auto Loan Asset Backed 
+ Notes (the “  Class B Notes  ”), Class C 5.36% Auto Loan  Asset Backed Notes (the “  Class C Notes  ”) and Class  D 6.34% Auto Loan Asset Backed 
+ Notes (the “  Class D Notes  ”, and together with the  Class A-1 Notes, the Class A-2 Notes, the Class A-3 Notes, the Class A-4 Notes, the Class B Notes 
+ and the Class C Notes, the “  Notes  ”). 
+ GRANTING CLAUSE 
+ The Issuer , to secure the payment of principal of and interest on, and any other amounts owing in respect of, the Notes equally and ratably 
+ without prejudice, priority or distinction except as set forth herein, and to secure compliance with the provisions of this Indenture, hereby Grants in trust 
+ to the Indenture T rustee on the Closing Date, as trustee for the benefit of the Noteholders, all of the Issuer ’s right, title and interest, whether now owned 
+ or hereafter acquired, in and to (i) the T rust Estate and (ii) all present and future claims, demands, causes and choses in action in respect of any or all of 
+ the T rust Estate and all payments on or under and all proceeds of every kind and nature whatsoever in respect of any or all of the T rust Estate, including 
+ all proceeds of the conversion, voluntary or involuntary , into cash or other liquid property , all cash proceeds, accounts, accounts receivable, notes, drafts, 
+ acceptances, chattel paper , checks, deposit accounts, insurance proceeds, condemnation awards, rights to payment of any and every kind and other forms 
+ of obligations and receivables, instruments, securities, financial assets and other property which at any time constitute all or part of or are included in the 
+ proceeds of any of the T rust Estate (collectively , the “  Collateral  ”). 
+ The Indenture T rustee, on behalf of the Noteholders, acknowledges the foregoing Grant, accepts the trusts under this Indenture and 
+ agrees to perform its duties required in this Indenture in accordance with the provisions of this Indenture. 
+ The foregoing Grant is made in trust to secure (i) the payment of principal of and interest on, and any other amounts owing in respect of, 
+ the Notes, equally and ratably without prejudice, priority or distinction except as set forth herein and (ii) compliance with the provisions of this 
+ Indenture, all as provided in this Indenture. 
+ Without limiting the foregoing Grant, any Receivable repurchased or purchased by (a) the Servicer pursuant to  Section 3.6  of the Servicing 
+ Agreement or (b) by the Bank pursuant to  Section 3.4  of the Purchase Agreement shall be deemed to be automatically released from the lien of this 
+ Indenture without any action being taken by the Indenture T rustee upon payment by the applicable purchaser of the related Repurchase Price for such 
+ Repurchased Receivable. 
+ COPAR 2023-1 Indentur e 
+--- [START OF PAGE 12] ---
+ ARTICLE I 
+ DEFINITIONS AND INCORPORA TION BY REFERENCE 
+ SECTION 1.1  Definitions  . Capitalized terms are used  in this Indenture as defined in  A  p  p  endix A  to the  Sale Agreement, dated as of the 
+ date hereof (as amended, supplemented, or otherwise modified and in ef fect from time to time, the “  Sale  Agreement  ”), between the Issuer and Capital 
+ One Auto Receivables, LLC, which also contains rules as to usage that are applicable herein. 
+ SECTION 1.2  Incorporation by Reference of T rust Indenture  Act  . Whenever this Indenture refers to a provision  of the TIA, the provision 
+ is incorporated by reference in and made a part of this Indenture. The following TIA terms used in this Indenture have the following meanings: 
+ “  Commission  ” means the Securities and Exchange Commission. 
+ “  indenture securities  ” means the Notes. 
+ “  indenture securi  ty  holder  ” means a Noteholder . 
+ “  indenture to be qualified  ” means this Indenture. 
+ “  indenture trustee  ” or “  institutional trustee  ” means  the Indenture T rustee. 
+ “  obl  ig  or  ” on the indenture securities means the Issuer  and any other obligor on the indenture securities. 
+ All other TIA terms used in this Indenture that are defined by the TIA, defined by TIA reference to another statute or defined by 
+ Commission rule have the meaning assigned to them by such definitions. 
+ SECTION 1.3  Other Interpretive Provisions  . All terms  defined in this Indenture shall have the defined meanings when used in any 
+ certificate or other document delivered pursuant hereto unless otherwise defined therein. For purposes of this Indenture and all such certificates and 
+ other documents, unless the context otherwise requires: (a) accounting terms not otherwise defined in this Indenture, and accounting terms partly 
+ defined in this Indenture to the extent not defined, shall have the respective meanings given to them under GAAP (  provided  , that, to the extent that the 
+ definitions in this Indenture and GAAP conflict, the definitions in this Indenture shall control); (b) terms defined in Article 9 of the UCC as in ef fect in 
+ the relevant jurisdiction and not otherwise defined in this Indenture are used as defined in that Article; (c) the words “hereof,” “herein” and “hereunder” 
+ and words of similar import refer to this Indenture as a whole and not to any particular provision of this Indenture; (d) references to any Article, 
+ Section, Schedule, Appendix or Exhibit are references to Articles, Sections, Schedules, Appendices and Exhibits in or to this Indenture and references 
+ to any paragraph, subsection, clause or other subdivision within any Section or definition refer to such paragraph, subsection, clause or other 
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 11, Paragraph 1",
+      "error": "Typographical error in the name 'CAPITAL ONE PRIME AUTO RECEIVABLES TRUST 2023-1'.",
+      "suggestion": "Correct the typographical error to 'CAPITAL ONE PRIME AUTO RECEIVABLES TRUST 2023-1'.",
+      "exact_quote": "CAPIT AL ONE PRIME AUT O RECEIV ABLES TRUST 2023-1"
+    },
+    {
+      "location": "Page 1, Exhibit Title",
+      "error": "Typographical errors in exhibit title and names.",
+      "suggestion": "Correct 'CAPIT AL ONE PRIME AUT O RECEIV ABLES TRUST 2023-1' to 'CAPITAL ONE PRIME AUTO RECEIVABLES TRUST 2023-1', and 'INDENTURE' to ensure consistency.",
+      "exact_quote": "CAPIT AL ONE PRIME AUT O RECEIV ABLES TRUST 2023-1"
+    },
+    {
+      "location": "Page 2, Cross Reference Table",
+      "error": "Typographical errors in section title.",
+      "suggestion": "Correct 'CROSS REFERENCE T ABLE' to 'CROSS REFERENCE TABLE'.",
+      "exact_quote": "CROSS REFERENCE T ABLE"
+    },
+    {
+      "location": "Page 10, Section 11.14",
+      "error": "Typographical error in section heading 'GOVERNING LA W'.",
+      "suggestion": "Correct 'GOVERNING LA W' to 'GOVERNING LAW'.",
+      "exact_quote": "GOVERNING LA W"
+    },
+    {
+      "location": "Page 11, Article I Section 1.1",
+      "error": "Typographical error in word 'Appendix'.",
+      "suggestion": "Correct 'A p p endix A' to 'Appendix A'.",
+      "exact_quote": "A p p endix A"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-30 15:44:44</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>gemini-2.5-flash</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>226ad1f9-61fe-40e1-9bc5-811645dabfda.pdf</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document f...</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Role: You are a strict, pedantic Legal Proofreader. You are reviewing a standalone legal document fragment.
+Input: The attached text from a contract.
+CRITICAL INSTRUCTIONS:
+1. **Assume Isolation with Common Sense**: Do NOT assume missing definitions exist in other documents. However, IGNORE common commercial lending terms typically defined in a base Credit Agreement (e.g., "Borrower", "Administrative Agent", "Lender", "Business Day", "Dollars", "GAAP", "Material Adverse Effect"). Only flag specific, deal-specific, or unusual capitalized terms that are undefined.
+2. **Logic Check:** Check all math and logic tables.
+3. **Drafting Errors:** Find any placeholders like "[__]" or blank lines that were forgotten.
+4. **Exact Quotes:** For every error, you MUST provide the `exact_quote` from the text that contains the error. This is used for highlighting.
+Output Format:
+Return ONLY a valid JSON object with the following structure:
+{
+  "errors": [
+    {
+      "location": "Page 3, Section 2.1",
+      "error": "Description of the error",
+      "suggestion": "Suggested fix",
+      "exact_quote": "Exact text substring to highlight in red"
+    }
+  ]
+}
+If no errors are found, return {"errors": []}.
+--- CONTRACT TEXT BEGINS ---
+--- [START OF PAGE 1] ---
+FIRST AMENDMENT TO AMENDED AND RESTATED
+CREDIT AGREEMENT
+This document is a generated test file containing intentional legal drafting errors for AI training
+purposes.
+ARTICLE I: DEFINITIONS
+...
+"Applicable Margin" means the corresponding percentages per annum as set forth below based on
+the Consolidated Total Leverage Ratio:
+Pricing Level
+Consolidated Total Leverage Ratio
+SOFR Margin
+I
+Greater than or equal to 3.25 to 1.00
+2.75%
+II
+Greater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00
+2.50%
+III
+Greater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00
+2.25%
+IV
+Greater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00
+2.00%
+V
+Less than 1.50 to 1.00
+1.75%
+"Cash Collateral" shall have a meaning correlative to the foregoing and shall include the proceeds of
+such cash collateral...
+(Note: "Cash Collateralize" is defined, but "Cash Collateralization" is NOT defined
+in this section.)
+SECTION 2.5 Permanent Reduction of the Revolving Credit
+Commitment
+The Borrower shall have the right at any time to terminate the Revolving Credit Commitment...
+Any reduction of the Revolving Credit Commitment to zero shall be accompanied by payment of all
+outstanding Revolving Credit Loans and furnishing of Cash Collateralization satisfactory to the
+Administrative Agent.
+SECTION 5.13 Incremental Loans
+At any time after the First Amendment Effective Date, the Borrower may by written notice to the
+Administrative Agent elect to request the establishment of one or more increases in the Revolving
+--- [START OF PAGE 2] ---
+Credit Commitments...
+Such notice shall be delivered to the Administrative Agent at its office in [__] (or such other location as
+the Administrative Agent may designate).
+The terms of such Incremental Revolving Credit Increase shall be subject to the documentation
+requirements set forth in Section 5.19.
+[End of Document]
+--- CONTRACT TEXT ENDS ---</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>{
+  "errors": [
+    {
+      "location": "Page 1, ARTICLE I: DEFINITIONS",
+      "error": "There is a logical gap in the 'Consolidated Total Leverage Ratio' ranges for the 'Applicable Margin' definition. Specifically, ratios greater than or equal to 2.50 to 1.00 but less than 2.60 to 1.00 are not covered by any pricing level, as Level III ends at 'less than 2.50 to 1.00' and Level II begins at 'Greater than or equal to 2.60 to 1.00'.",
+      "suggestion": "Adjust the ranges for Pricing Levels II and III to ensure continuous coverage without gaps, for example, by changing Level III to 'Greater than or equal to 1.75 to 1.00 but less than 2.60 to 1.00' or by changing Level II to 'Greater than or equal to 2.50 to 1.00 but less than 3.25 to 1.00'.",
+      "exact_quote": "Pricing Level\nConsolidated Total Leverage Ratio\nSOFR Margin\nI\nGreater than or equal to 3.25 to 1.00\n2.75%\nII\nGreater than or equal to 2.60 to 1.00 but less than 3.25 to 1.00\n2.50%\nIII\nGreater than or equal to 1.75 to 1.00 but less than 2.50 to 1.00\n2.25%\nIV\nGreater than or equal to 1.50 to 1.00 but less than 1.75 to 1.00\n2.00%\nV\nLess than 1.50 to 1.00\n1.75%"
+    },
+    {
+      "location": "Page 1, SECTION 2.5",
+      "error": "The capitalized term 'Cash Collateralization' is used but not defined in this document fragment. It is a deal-specific term requiring definition.",
+      "suggestion": "Add a definition for 'Cash Collateralization' in ARTICLE I or replace it with an already defined term if one exists that conveys the same meaning.",
+      "exact_quote": "Cash Collateralization"
+    },
+    {
+      "location": "Page 1, SECTION 5.13",
+      "error": "The capitalized term 'First Amendment Effective Date' is used but not defined in this document fragment. This is a critical, deal-specific term that requires a definition.",
+      "suggestion": "Add a definition for 'First Amendment Effective Date' in ARTICLE I.",
+      "exact_quote": "First Amendment Effective Date"
+    },
+    {
+      "location": "Page 2, SECTION 5.13",
+      "error": "A placeholder '[__]' has been left in the text, indicating missing information for the Administrative Agent's office location.",
+      "suggestion": "Replace '[__]' with the specific office location of the Administrative Agent.",
+      "exact_quote": "[__]"
+    }
+  ]
+}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>